<commit_message>
Add in .gitignore file for temporary Excel files.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1200" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3440" yWindow="7220" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
     <sheet name="FIS Recommendation" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="214">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -659,13 +659,16 @@
   </si>
   <si>
     <t>Watched?</t>
+  </si>
+  <si>
+    <t>Dynamic find_by Methods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -675,6 +678,18 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -701,8 +716,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -718,51 +735,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1091,11 +1069,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D432"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1133,6 +1111,12 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="3">
+        <v>41521</v>
+      </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1">
@@ -3276,6 +3260,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3288,7 +3273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Watch additional RailsCasts on model associations in controllers.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="7220" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="3120" yWindow="1580" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="215">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -662,6 +662,9 @@
   </si>
   <si>
     <t>Dynamic find_by Methods</t>
+  </si>
+  <si>
+    <t>Find Through Association</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -735,9 +740,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,14 +1080,14 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="35.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1121,6 +1128,12 @@
     <row r="5" spans="2:4">
       <c r="B5" s="1">
         <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="3">
+        <v>41521</v>
       </c>
     </row>
     <row r="6" spans="2:4">

</xml_diff>

<commit_message>
Add comments column to all RailsCasts and watchd RailsCast 4.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="221">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -665,6 +665,24 @@
   </si>
   <si>
     <t>Find Through Association</t>
+  </si>
+  <si>
+    <t>Move Find into Model</t>
+  </si>
+  <si>
+    <t>Quick Summary</t>
+  </si>
+  <si>
+    <t>Use of memoziation (||=) when caching instance variables in models (e.g. authentication).</t>
+  </si>
+  <si>
+    <t>Use of &lt;model&gt;.find_by_&lt;attribute&gt;(&lt;condition&gt;) is powerful syntax.</t>
+  </si>
+  <si>
+    <t>Dynamic find_by can be used through rails model associations.</t>
+  </si>
+  <si>
+    <t>Repetetive finds (with specific queries) should be moved into model space.</t>
   </si>
 </sst>
 </file>
@@ -726,7 +744,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -738,6 +756,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1074,13 +1098,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D432"/>
+  <dimension ref="B1:E432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1088,11 +1112,13 @@
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="75.83203125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="10" customHeight="1"/>
-    <row r="2" spans="2:4">
+    <row r="1" spans="2:5" ht="10" customHeight="1"/>
+    <row r="2" spans="2:5">
       <c r="B2" s="2" t="s">
         <v>210</v>
       </c>
@@ -1102,8 +1128,11 @@
       <c r="D2" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="E2" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1113,8 +1142,11 @@
       <c r="D3" s="3">
         <v>41521</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="E3" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1124,8 +1156,11 @@
       <c r="D4" s="3">
         <v>41521</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="E4" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1135,58 +1170,70 @@
       <c r="D5" s="3">
         <v>41521</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="E5" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="C6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="4">
+        <v>41524</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:5">
       <c r="B8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:5">
       <c r="B9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:5">
       <c r="B10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:5">
       <c r="B11" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:5">
       <c r="B12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:5">
       <c r="B13" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:5">
       <c r="B14" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:5">
       <c r="B15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:5">
       <c r="B16" s="1">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Watch RailsCast 320 on Jbuilder.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="1580" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
@@ -10,6 +10,9 @@
     <sheet name="List" sheetId="2" r:id="rId1"/>
     <sheet name="FIS Recommendation" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$E$432</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="223">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -683,6 +686,12 @@
   </si>
   <si>
     <t>Repetetive finds (with specific queries) should be moved into model space.</t>
+  </si>
+  <si>
+    <t>Jbuilder</t>
+  </si>
+  <si>
+    <t>Jbuilder is used to create custom JSON objects via DSL for Rails models.</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1113,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1190,1582 +1199,1591 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1">
-        <v>5</v>
+        <v>320</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="4">
+        <v>41548</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="1">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="1">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" s="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" s="1">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" s="1">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="1">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="1">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="1">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="1">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" s="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" s="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="1">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="1">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" s="1">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" s="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" s="1">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" s="1">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" s="1">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" s="1">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" s="1">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="1">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" s="1">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" s="1">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" s="1">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" s="1">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" s="1">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" s="1">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" s="1">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" s="1">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" s="1">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" s="1">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" s="1">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" s="1">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" s="1">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" s="1">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" s="1">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" s="1">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" s="1">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" s="1">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" s="1">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" s="1">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" s="1">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" s="1">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" s="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" s="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" s="1">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" s="1">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" s="1">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" s="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" s="1">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" s="1">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" s="1">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" s="1">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" s="1">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" s="1">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" s="1">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" s="1">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" s="1">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" s="1">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" s="1">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" s="1">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" s="1">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" s="1">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" s="1">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" s="1">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" s="1">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" s="1">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" s="1">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" s="1">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" s="1">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" s="1">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" s="1">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" s="1">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" s="1">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" s="1">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" s="1">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" s="1">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" s="1">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" s="1">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" s="1">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" s="1">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" s="1">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" s="1">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" s="1">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" s="1">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" s="1">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" s="1">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" s="1">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" s="1">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" s="1">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" s="1">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" s="1">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" s="1">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" s="1">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" s="1">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" s="1">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" s="1">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" s="1">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" s="1">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" s="1">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" s="1">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" s="1">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" s="1">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" s="1">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" s="1">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" s="1">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" s="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" s="1">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" s="1">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" s="1">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" s="1">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" s="1">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" s="1">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" s="1">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="273" spans="2:2">
       <c r="B273" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="274" spans="2:2">
       <c r="B274" s="1">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="275" spans="2:2">
       <c r="B275" s="1">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="276" spans="2:2">
       <c r="B276" s="1">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="277" spans="2:2">
       <c r="B277" s="1">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="278" spans="2:2">
       <c r="B278" s="1">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="279" spans="2:2">
       <c r="B279" s="1">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="280" spans="2:2">
       <c r="B280" s="1">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="281" spans="2:2">
       <c r="B281" s="1">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" s="1">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" s="1">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" s="1">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="285" spans="2:2">
       <c r="B285" s="1">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="286" spans="2:2">
       <c r="B286" s="1">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="287" spans="2:2">
       <c r="B287" s="1">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="288" spans="2:2">
       <c r="B288" s="1">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" s="1">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" s="1">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" s="1">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" s="1">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" s="1">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" s="1">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" s="1">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" s="1">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" s="1">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" s="1">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" s="1">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" s="1">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" s="1">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" s="1">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" s="1">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="305" spans="2:2">
       <c r="B305" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="306" spans="2:2">
       <c r="B306" s="1">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="307" spans="2:2">
       <c r="B307" s="1">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="308" spans="2:2">
       <c r="B308" s="1">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="309" spans="2:2">
       <c r="B309" s="1">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="310" spans="2:2">
       <c r="B310" s="1">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="311" spans="2:2">
       <c r="B311" s="1">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="312" spans="2:2">
       <c r="B312" s="1">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="313" spans="2:2">
       <c r="B313" s="1">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="314" spans="2:2">
       <c r="B314" s="1">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="315" spans="2:2">
       <c r="B315" s="1">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="316" spans="2:2">
       <c r="B316" s="1">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="317" spans="2:2">
       <c r="B317" s="1">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="318" spans="2:2">
       <c r="B318" s="1">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="319" spans="2:2">
       <c r="B319" s="1">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="320" spans="2:2">
       <c r="B320" s="1">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="321" spans="2:2">
       <c r="B321" s="1">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="322" spans="2:2">
       <c r="B322" s="1">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="323" spans="2:2">
@@ -3319,6 +3337,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:E432">
+    <sortState ref="B3:E432">
+      <sortCondition ref="D2:D432"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Watch RailsCast 275: How I Test.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="225">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t>Jbuilder is used to create custom JSON objects via DSL for Rails models.</t>
+  </si>
+  <si>
+    <t>How I Test</t>
+  </si>
+  <si>
+    <t>Workflow of TDD using Rspec, Capybara, Factory Girl, and Girl w/ password reset link.</t>
   </si>
 </sst>
 </file>
@@ -753,7 +759,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -771,6 +777,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1110,10 +1119,10 @@
   <dimension ref="B1:E432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="E279" sqref="E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2536,82 +2545,91 @@
         <v>269</v>
       </c>
     </row>
-    <row r="273" spans="2:2">
+    <row r="273" spans="2:5">
       <c r="B273" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="274" spans="2:2">
+    <row r="274" spans="2:5">
       <c r="B274" s="1">
         <v>271</v>
       </c>
     </row>
-    <row r="275" spans="2:2">
+    <row r="275" spans="2:5">
       <c r="B275" s="1">
         <v>272</v>
       </c>
     </row>
-    <row r="276" spans="2:2">
+    <row r="276" spans="2:5">
       <c r="B276" s="1">
         <v>273</v>
       </c>
     </row>
-    <row r="277" spans="2:2">
+    <row r="277" spans="2:5">
       <c r="B277" s="1">
         <v>274</v>
       </c>
     </row>
-    <row r="278" spans="2:2">
+    <row r="278" spans="2:5">
       <c r="B278" s="1">
         <v>275</v>
       </c>
-    </row>
-    <row r="279" spans="2:2">
+      <c r="C278" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D278" s="6">
+        <v>41549</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="279" spans="2:5">
       <c r="B279" s="1">
         <v>276</v>
       </c>
     </row>
-    <row r="280" spans="2:2">
+    <row r="280" spans="2:5">
       <c r="B280" s="1">
         <v>277</v>
       </c>
     </row>
-    <row r="281" spans="2:2">
+    <row r="281" spans="2:5">
       <c r="B281" s="1">
         <v>278</v>
       </c>
     </row>
-    <row r="282" spans="2:2">
+    <row r="282" spans="2:5">
       <c r="B282" s="1">
         <v>279</v>
       </c>
     </row>
-    <row r="283" spans="2:2">
+    <row r="283" spans="2:5">
       <c r="B283" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="284" spans="2:2">
+    <row r="284" spans="2:5">
       <c r="B284" s="1">
         <v>281</v>
       </c>
     </row>
-    <row r="285" spans="2:2">
+    <row r="285" spans="2:5">
       <c r="B285" s="1">
         <v>282</v>
       </c>
     </row>
-    <row r="286" spans="2:2">
+    <row r="286" spans="2:5">
       <c r="B286" s="1">
         <v>283</v>
       </c>
     </row>
-    <row r="287" spans="2:2">
+    <row r="287" spans="2:5">
       <c r="B287" s="1">
         <v>284</v>
       </c>
     </row>
-    <row r="288" spans="2:2">
+    <row r="288" spans="2:5">
       <c r="B288" s="1">
         <v>285</v>
       </c>

</xml_diff>

<commit_message>
Watch RailsCast 005 on with_scope method.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1580" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="227">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>Workflow of TDD using Rspec, Capybara, Factory Girl, and Girl w/ password reset link.</t>
+  </si>
+  <si>
+    <t>Using with_scope</t>
+  </si>
+  <si>
+    <t>Allows for find options {:k =&gt; v} to be passed in from ctrlr to model, autoinherits parameters.</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1125,10 @@
   <dimension ref="B1:E432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E279" sqref="E279"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1223,6 +1229,15 @@
     <row r="8" spans="2:5">
       <c r="B8" s="1">
         <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="4">
+        <v>41557</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="2:5">

</xml_diff>

<commit_message>
Watch RailsCast 238 - Mongoid.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="229">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -704,6 +704,12 @@
   </si>
   <si>
     <t>Allows for find options {:k =&gt; v} to be passed in from ctrlr to model, autoinherits parameters.</t>
+  </si>
+  <si>
+    <t>Mongoid</t>
+  </si>
+  <si>
+    <t>Showcase of Mongoid driver in Ruby for MongoDB - DB setup, design, and implementation.</t>
   </si>
 </sst>
 </file>
@@ -765,7 +771,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -783,9 +789,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1128,7 +1131,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1228,1423 +1231,1432 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="1">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D8" s="4">
-        <v>41557</v>
+        <v>41549</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="4">
+        <v>41557</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1">
-        <v>7</v>
+        <v>238</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="4">
+        <v>41575</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="1">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="1">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="1">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="1">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="1">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="1">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="1">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="1">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="1">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="1">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="1">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" s="1">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="1">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="1">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" s="1">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="1">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="1">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="1">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" s="1">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="1">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="1">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="1">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="1">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" s="1">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="1">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="1">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" s="1">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" s="1">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" s="1">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" s="1">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" s="1">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="1">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="1">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" s="1">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="1">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" s="1">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="1">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" s="1">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" s="1">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" s="1">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" s="1">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" s="1">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="1">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="1">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" s="1">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="1">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" s="1">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="1">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="1">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="1">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="1">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" s="1">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" s="1">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" s="1">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="1">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="1">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" s="1">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="1">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" s="1">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="1">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="1">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" s="1">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="1">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" s="1">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" s="1">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" s="1">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="1">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="1">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="1">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="1">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="1">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="1">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="1">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" s="1">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" s="1">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" s="1">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" s="1">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" s="1">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="1">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="1">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" s="1">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="1">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" s="1">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="1">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="1">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" s="1">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" s="1">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" s="1">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" s="1">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" s="1">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" s="1">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" s="1">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" s="1">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" s="1">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" s="1">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="1">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" s="1">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" s="1">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" s="1">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" s="1">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" s="1">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" s="1">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" s="1">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" s="1">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" s="1">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" s="1">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" s="1">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" s="1">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" s="1">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" s="1">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" s="1">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" s="1">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" s="1">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" s="1">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" s="1">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" s="1">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" s="1">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" s="1">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" s="1">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" s="1">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" s="1">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" s="1">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" s="1">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" s="1">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" s="1">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" s="1">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" s="1">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" s="1">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" s="1">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" s="1">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" s="1">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" s="1">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" s="1">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" s="1">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" s="1">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" s="1">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" s="1">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" s="1">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" s="1">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" s="1">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" s="1">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" s="1">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" s="1">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" s="1">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" s="1">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" s="1">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" s="1">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" s="1">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" s="1">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" s="1">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" s="1">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" s="1">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" s="1">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" s="1">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" s="1">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" s="1">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" s="1">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" s="1">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="225" spans="2:2">
       <c r="B225" s="1">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" s="1">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="227" spans="2:2">
       <c r="B227" s="1">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="228" spans="2:2">
       <c r="B228" s="1">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="229" spans="2:2">
       <c r="B229" s="1">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="230" spans="2:2">
       <c r="B230" s="1">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="231" spans="2:2">
       <c r="B231" s="1">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="232" spans="2:2">
       <c r="B232" s="1">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="233" spans="2:2">
       <c r="B233" s="1">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="234" spans="2:2">
       <c r="B234" s="1">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="235" spans="2:2">
       <c r="B235" s="1">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="236" spans="2:2">
       <c r="B236" s="1">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="237" spans="2:2">
       <c r="B237" s="1">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" s="1">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" s="1">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="240" spans="2:2">
       <c r="B240" s="1">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" s="1">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" s="1">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" s="1">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" s="1">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" s="1">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" s="1">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" s="1">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" s="1">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" s="1">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" s="1">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" s="1">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" s="1">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" s="1">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" s="1">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" s="1">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" s="1">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" s="1">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" s="1">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" s="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" s="1">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" s="1">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" s="1">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" s="1">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" s="1">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" s="1">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" s="1">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" s="1">
         <v>269</v>
       </c>
     </row>
-    <row r="273" spans="2:5">
-      <c r="B273" s="1">
+    <row r="274" spans="2:2">
+      <c r="B274" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="274" spans="2:5">
-      <c r="B274" s="1">
+    <row r="275" spans="2:2">
+      <c r="B275" s="1">
         <v>271</v>
       </c>
     </row>
-    <row r="275" spans="2:5">
-      <c r="B275" s="1">
+    <row r="276" spans="2:2">
+      <c r="B276" s="1">
         <v>272</v>
       </c>
     </row>
-    <row r="276" spans="2:5">
-      <c r="B276" s="1">
+    <row r="277" spans="2:2">
+      <c r="B277" s="1">
         <v>273</v>
       </c>
     </row>
-    <row r="277" spans="2:5">
-      <c r="B277" s="1">
+    <row r="278" spans="2:2">
+      <c r="B278" s="1">
         <v>274</v>
       </c>
     </row>
-    <row r="278" spans="2:5">
-      <c r="B278" s="1">
-        <v>275</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D278" s="6">
-        <v>41549</v>
-      </c>
-      <c r="E278" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="279" spans="2:5">
+    <row r="279" spans="2:2">
       <c r="B279" s="1">
         <v>276</v>
       </c>
     </row>
-    <row r="280" spans="2:5">
+    <row r="280" spans="2:2">
       <c r="B280" s="1">
         <v>277</v>
       </c>
     </row>
-    <row r="281" spans="2:5">
+    <row r="281" spans="2:2">
       <c r="B281" s="1">
         <v>278</v>
       </c>
     </row>
-    <row r="282" spans="2:5">
+    <row r="282" spans="2:2">
       <c r="B282" s="1">
         <v>279</v>
       </c>
     </row>
-    <row r="283" spans="2:5">
+    <row r="283" spans="2:2">
       <c r="B283" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="284" spans="2:5">
+    <row r="284" spans="2:2">
       <c r="B284" s="1">
         <v>281</v>
       </c>
     </row>
-    <row r="285" spans="2:5">
+    <row r="285" spans="2:2">
       <c r="B285" s="1">
         <v>282</v>
       </c>
     </row>
-    <row r="286" spans="2:5">
+    <row r="286" spans="2:2">
       <c r="B286" s="1">
         <v>283</v>
       </c>
     </row>
-    <row r="287" spans="2:5">
+    <row r="287" spans="2:2">
       <c r="B287" s="1">
         <v>284</v>
       </c>
     </row>
-    <row r="288" spans="2:5">
+    <row r="288" spans="2:2">
       <c r="B288" s="1">
         <v>285</v>
       </c>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 006, 007.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="9400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="233">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -710,6 +710,18 @@
   </si>
   <si>
     <t>Showcase of Mongoid driver in Ruby for MongoDB - DB setup, design, and implementation.</t>
+  </si>
+  <si>
+    <t>Shorcut Blocks w/ Symbol to_proc</t>
+  </si>
+  <si>
+    <t>Use of (&amp;:notation) when using blocks [ e.g. projects.collect(&amp;:name).collect(&amp;:downcase) ]</t>
+  </si>
+  <si>
+    <t>Layouts</t>
+  </si>
+  <si>
+    <t>Priority: Controller Action Render &gt;&gt; In-Line Controller &gt;&gt; Controller &gt;&gt; Application</t>
   </si>
 </sst>
 </file>
@@ -741,18 +753,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -771,7 +777,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -781,14 +787,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1131,7 +1140,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1140,7 +1149,7 @@
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="75.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="75.83203125" style="3" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1166,10 +1175,10 @@
       <c r="C3" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>41521</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1180,10 +1189,10 @@
       <c r="C4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>41521</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>218</v>
       </c>
     </row>
@@ -1194,10 +1203,10 @@
       <c r="C5" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>41521</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -1208,1695 +1217,1713 @@
       <c r="C6" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>41524</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1">
-        <v>320</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" s="4">
-        <v>41548</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>222</v>
+        <v>225</v>
+      </c>
+      <c r="D7" s="6">
+        <v>41557</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="1">
-        <v>275</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D8" s="4">
-        <v>41549</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>224</v>
+        <v>41974</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D9" s="4">
-        <v>41557</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>226</v>
+        <v>41974</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1">
-        <v>238</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="4">
-        <v>41575</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="1">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="1">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="1">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="1">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="1">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="1">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="1">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" s="1">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="1">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" s="1">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="1">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="1">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="1">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="1">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="1">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64" s="1">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70" s="1">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71" s="1">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="1">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="1">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="1">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75" s="1">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="1">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="1">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="1">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" s="1">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="1">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="1">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="1">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" s="1">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="1">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="1">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="1">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="1">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" s="1">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="1">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="1">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" s="1">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" s="1">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" s="1">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" s="1">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" s="1">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="1">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="1">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" s="1">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="1">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" s="1">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="1">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="1">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" s="1">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" s="1">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" s="1">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108" s="1">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="1">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="1">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="2:2">
       <c r="B111" s="1">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="1">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:2">
       <c r="B113" s="1">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="1">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="1">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="1">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="1">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="2:2">
       <c r="B118" s="1">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="2:2">
       <c r="B119" s="1">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="2:2">
       <c r="B120" s="1">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="1">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="1">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="2:2">
       <c r="B123" s="1">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="1">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="2:2">
       <c r="B125" s="1">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="1">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="1">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="2:2">
       <c r="B128" s="1">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="1">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="2:2">
       <c r="B130" s="1">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="2:2">
       <c r="B131" s="1">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="2:2">
       <c r="B132" s="1">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="1">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="1">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="2:2">
       <c r="B135" s="1">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="1">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" s="1">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="1">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="1">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="2:2">
       <c r="B140" s="1">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="2:2">
       <c r="B141" s="1">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="2:2">
       <c r="B142" s="1">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="2:2">
       <c r="B143" s="1">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="2:2">
       <c r="B144" s="1">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="1">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="1">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="2:2">
       <c r="B147" s="1">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="1">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" s="1">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="1">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="1">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="2:2">
       <c r="B152" s="1">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" s="1">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" s="1">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" s="1">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="2:2">
       <c r="B156" s="1">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="2:2">
       <c r="B157" s="1">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="2:2">
       <c r="B158" s="1">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="2:2">
       <c r="B159" s="1">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="2:2">
       <c r="B160" s="1">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="2:2">
       <c r="B161" s="1">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="1">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="2:2">
       <c r="B163" s="1">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="2:2">
       <c r="B164" s="1">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="2:2">
       <c r="B165" s="1">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="166" spans="2:2">
       <c r="B166" s="1">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="167" spans="2:2">
       <c r="B167" s="1">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" s="1">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="2:2">
       <c r="B169" s="1">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="2:2">
       <c r="B170" s="1">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" s="1">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" s="1">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="2:2">
       <c r="B173" s="1">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="2:2">
       <c r="B174" s="1">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="175" spans="2:2">
       <c r="B175" s="1">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="2:2">
       <c r="B176" s="1">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="2:2">
       <c r="B177" s="1">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="2:2">
       <c r="B178" s="1">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="2:2">
       <c r="B179" s="1">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="2:2">
       <c r="B180" s="1">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="181" spans="2:2">
       <c r="B181" s="1">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="2:2">
       <c r="B182" s="1">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="2:2">
       <c r="B183" s="1">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="2:2">
       <c r="B184" s="1">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="2:2">
       <c r="B185" s="1">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="186" spans="2:2">
       <c r="B186" s="1">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="187" spans="2:2">
       <c r="B187" s="1">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="2:2">
       <c r="B188" s="1">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="189" spans="2:2">
       <c r="B189" s="1">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="190" spans="2:2">
       <c r="B190" s="1">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="191" spans="2:2">
       <c r="B191" s="1">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="192" spans="2:2">
       <c r="B192" s="1">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="193" spans="2:2">
       <c r="B193" s="1">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="194" spans="2:2">
       <c r="B194" s="1">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" s="1">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" s="1">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="197" spans="2:2">
       <c r="B197" s="1">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="198" spans="2:2">
       <c r="B198" s="1">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="2:2">
       <c r="B199" s="1">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="2:2">
       <c r="B200" s="1">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="201" spans="2:2">
       <c r="B201" s="1">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="202" spans="2:2">
       <c r="B202" s="1">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="203" spans="2:2">
       <c r="B203" s="1">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="2:2">
       <c r="B204" s="1">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="205" spans="2:2">
       <c r="B205" s="1">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="2:2">
       <c r="B206" s="1">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="207" spans="2:2">
       <c r="B207" s="1">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="208" spans="2:2">
       <c r="B208" s="1">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="209" spans="2:2">
       <c r="B209" s="1">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="210" spans="2:2">
       <c r="B210" s="1">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="211" spans="2:2">
       <c r="B211" s="1">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="212" spans="2:2">
       <c r="B212" s="1">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="213" spans="2:2">
       <c r="B213" s="1">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="214" spans="2:2">
       <c r="B214" s="1">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="215" spans="2:2">
       <c r="B215" s="1">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="216" spans="2:2">
       <c r="B216" s="1">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="217" spans="2:2">
       <c r="B217" s="1">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="2:2">
       <c r="B218" s="1">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="219" spans="2:2">
       <c r="B219" s="1">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" s="1">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" s="1">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="222" spans="2:2">
       <c r="B222" s="1">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="223" spans="2:2">
       <c r="B223" s="1">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="224" spans="2:2">
       <c r="B224" s="1">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="225" spans="2:2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="2:5">
       <c r="B225" s="1">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="226" spans="2:2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="2:5">
       <c r="B226" s="1">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="227" spans="2:2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="2:5">
       <c r="B227" s="1">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="228" spans="2:2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="2:5">
       <c r="B228" s="1">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="229" spans="2:2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="2:5">
       <c r="B229" s="1">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="230" spans="2:2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="2:5">
       <c r="B230" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="231" spans="2:2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="2:5">
       <c r="B231" s="1">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="232" spans="2:2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="2:5">
       <c r="B232" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="2:5">
+      <c r="B233" s="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="2:5">
+      <c r="B234" s="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="2:5">
+      <c r="B235" s="1">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="2:5">
+      <c r="B236" s="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="2:5">
+      <c r="B237" s="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" spans="2:5">
+      <c r="B238" s="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="2:5">
+      <c r="B239" s="1">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="240" spans="2:5">
+      <c r="B240" s="1">
+        <v>238</v>
+      </c>
+      <c r="C240" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="233" spans="2:2">
-      <c r="B233" s="1">
+      <c r="D240" s="6">
+        <v>41575</v>
+      </c>
+      <c r="E240" s="3" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="234" spans="2:2">
-      <c r="B234" s="1">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="235" spans="2:2">
-      <c r="B235" s="1">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="236" spans="2:2">
-      <c r="B236" s="1">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="237" spans="2:2">
-      <c r="B237" s="1">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="238" spans="2:2">
-      <c r="B238" s="1">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="239" spans="2:2">
-      <c r="B239" s="1">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="240" spans="2:2">
-      <c r="B240" s="1">
-        <v>235</v>
       </c>
     </row>
     <row r="241" spans="2:2">
       <c r="B241" s="1">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="242" spans="2:2">
       <c r="B242" s="1">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" s="1">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" s="1">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" s="1">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" s="1">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" s="1">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" s="1">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" s="1">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" s="1">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" s="1">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="252" spans="2:2">
       <c r="B252" s="1">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="253" spans="2:2">
       <c r="B253" s="1">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" s="1">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" s="1">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" s="1">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="257" spans="2:2">
       <c r="B257" s="1">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="258" spans="2:2">
       <c r="B258" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="259" spans="2:2">
       <c r="B259" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="260" spans="2:2">
       <c r="B260" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" s="1">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="262" spans="2:2">
       <c r="B262" s="1">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="263" spans="2:2">
       <c r="B263" s="1">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" s="1">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="265" spans="2:2">
       <c r="B265" s="1">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" s="1">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="267" spans="2:2">
       <c r="B267" s="1">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="268" spans="2:2">
       <c r="B268" s="1">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" s="1">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="270" spans="2:2">
       <c r="B270" s="1">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="271" spans="2:2">
       <c r="B271" s="1">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="272" spans="2:2">
       <c r="B272" s="1">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="273" spans="2:2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="273" spans="2:5">
       <c r="B273" s="1">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="274" spans="2:2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="274" spans="2:5">
       <c r="B274" s="1">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="275" spans="2:2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="275" spans="2:5">
       <c r="B275" s="1">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="276" spans="2:2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="276" spans="2:5">
       <c r="B276" s="1">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="277" spans="2:2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="277" spans="2:5">
       <c r="B277" s="1">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="278" spans="2:2">
+        <v>275</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D277" s="6">
+        <v>41549</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="278" spans="2:5">
       <c r="B278" s="1">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="279" spans="2:2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="279" spans="2:5">
       <c r="B279" s="1">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="280" spans="2:2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="280" spans="2:5">
       <c r="B280" s="1">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="281" spans="2:2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="281" spans="2:5">
       <c r="B281" s="1">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="282" spans="2:2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="282" spans="2:5">
       <c r="B282" s="1">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="283" spans="2:2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5">
       <c r="B283" s="1">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="284" spans="2:2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="284" spans="2:5">
       <c r="B284" s="1">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="285" spans="2:2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="285" spans="2:5">
       <c r="B285" s="1">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="286" spans="2:2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="286" spans="2:5">
       <c r="B286" s="1">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="287" spans="2:2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="287" spans="2:5">
       <c r="B287" s="1">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="288" spans="2:2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="288" spans="2:5">
       <c r="B288" s="1">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="289" spans="2:2">
       <c r="B289" s="1">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="290" spans="2:2">
       <c r="B290" s="1">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="291" spans="2:2">
       <c r="B291" s="1">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="292" spans="2:2">
       <c r="B292" s="1">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="293" spans="2:2">
       <c r="B293" s="1">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="294" spans="2:2">
       <c r="B294" s="1">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="295" spans="2:2">
       <c r="B295" s="1">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="296" spans="2:2">
       <c r="B296" s="1">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="297" spans="2:2">
       <c r="B297" s="1">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="298" spans="2:2">
       <c r="B298" s="1">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" s="1">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="300" spans="2:2">
       <c r="B300" s="1">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="301" spans="2:2">
       <c r="B301" s="1">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="302" spans="2:2">
       <c r="B302" s="1">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" s="1">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="304" spans="2:2">
       <c r="B304" s="1">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="305" spans="2:2">
       <c r="B305" s="1">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="306" spans="2:2">
       <c r="B306" s="1">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="307" spans="2:2">
       <c r="B307" s="1">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="308" spans="2:2">
       <c r="B308" s="1">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="309" spans="2:2">
       <c r="B309" s="1">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="310" spans="2:2">
       <c r="B310" s="1">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="311" spans="2:2">
       <c r="B311" s="1">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="312" spans="2:2">
       <c r="B312" s="1">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="313" spans="2:2">
       <c r="B313" s="1">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="314" spans="2:2">
       <c r="B314" s="1">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="315" spans="2:2">
       <c r="B315" s="1">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="316" spans="2:2">
       <c r="B316" s="1">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="317" spans="2:2">
       <c r="B317" s="1">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="318" spans="2:2">
       <c r="B318" s="1">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="319" spans="2:2">
       <c r="B319" s="1">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="320" spans="2:2">
       <c r="B320" s="1">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="321" spans="2:2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="321" spans="2:5">
       <c r="B321" s="1">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="322" spans="2:2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5">
       <c r="B322" s="1">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="323" spans="2:2">
+        <v>320</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D322" s="6">
+        <v>41548</v>
+      </c>
+      <c r="E322" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="323" spans="2:5">
       <c r="B323" s="1">
         <v>321</v>
       </c>
     </row>
-    <row r="324" spans="2:2">
+    <row r="324" spans="2:5">
       <c r="B324" s="1">
         <v>322</v>
       </c>
     </row>
-    <row r="325" spans="2:2">
+    <row r="325" spans="2:5">
       <c r="B325" s="1">
         <v>323</v>
       </c>
     </row>
-    <row r="326" spans="2:2">
+    <row r="326" spans="2:5">
       <c r="B326" s="1">
         <v>324</v>
       </c>
     </row>
-    <row r="327" spans="2:2">
+    <row r="327" spans="2:5">
       <c r="B327" s="1">
         <v>325</v>
       </c>
     </row>
-    <row r="328" spans="2:2">
+    <row r="328" spans="2:5">
       <c r="B328" s="1">
         <v>326</v>
       </c>
     </row>
-    <row r="329" spans="2:2">
+    <row r="329" spans="2:5">
       <c r="B329" s="1">
         <v>327</v>
       </c>
     </row>
-    <row r="330" spans="2:2">
+    <row r="330" spans="2:5">
       <c r="B330" s="1">
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="2:2">
+    <row r="331" spans="2:5">
       <c r="B331" s="1">
         <v>329</v>
       </c>
     </row>
-    <row r="332" spans="2:2">
+    <row r="332" spans="2:5">
       <c r="B332" s="1">
         <v>330</v>
       </c>
     </row>
-    <row r="333" spans="2:2">
+    <row r="333" spans="2:5">
       <c r="B333" s="1">
         <v>331</v>
       </c>
     </row>
-    <row r="334" spans="2:2">
+    <row r="334" spans="2:5">
       <c r="B334" s="1">
         <v>332</v>
       </c>
     </row>
-    <row r="335" spans="2:2">
+    <row r="335" spans="2:5">
       <c r="B335" s="1">
         <v>333</v>
       </c>
     </row>
-    <row r="336" spans="2:2">
+    <row r="336" spans="2:5">
       <c r="B336" s="1">
         <v>334</v>
       </c>
@@ -3384,7 +3411,7 @@
   </sheetData>
   <autoFilter ref="B2:E432">
     <sortState ref="B3:E432">
-      <sortCondition ref="D2:D432"/>
+      <sortCondition ref="B2:B432"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixes row offsets for RailsCasts XLSX.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1134,13 +1134,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E432"/>
+  <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B410" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="B420" sqref="B420:B432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3341,71 +3341,6 @@
     <row r="419" spans="2:2">
       <c r="B419" s="1">
         <v>417</v>
-      </c>
-    </row>
-    <row r="420" spans="2:2">
-      <c r="B420" s="1">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="421" spans="2:2">
-      <c r="B421" s="1">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="422" spans="2:2">
-      <c r="B422" s="1">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="423" spans="2:2">
-      <c r="B423" s="1">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="424" spans="2:2">
-      <c r="B424" s="1">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="425" spans="2:2">
-      <c r="B425" s="1">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="426" spans="2:2">
-      <c r="B426" s="1">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="427" spans="2:2">
-      <c r="B427" s="1">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="428" spans="2:2">
-      <c r="B428" s="1">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="429" spans="2:2">
-      <c r="B429" s="1">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="430" spans="2:2">
-      <c r="B430" s="1">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="431" spans="2:2">
-      <c r="B431" s="1">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="432" spans="2:2">
-      <c r="B432" s="1">
-        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 008.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="235">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -722,6 +722,12 @@
   </si>
   <si>
     <t>Priority: Controller Action Render &gt;&gt; In-Line Controller &gt;&gt; Controller &gt;&gt; Application</t>
+  </si>
+  <si>
+    <t>Layouts and content_for</t>
+  </si>
+  <si>
+    <t>&lt;%= yield :head %&gt; in layout, &lt;% content_for :head do %&gt; … &lt;% end %&gt; in view</t>
   </si>
 </sst>
 </file>
@@ -770,8 +776,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -800,11 +808,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1137,10 +1147,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B410" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B420" sqref="B420:B432"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1269,6 +1279,15 @@
     <row r="10" spans="2:5">
       <c r="B10" s="1">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="4">
+        <v>41975</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 009, 010, 011, 012.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="0" windowWidth="14400" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="243">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -728,6 +728,30 @@
   </si>
   <si>
     <t>&lt;%= yield :head %&gt; in layout, &lt;% content_for :head do %&gt; … &lt;% end %&gt; in view</t>
+  </si>
+  <si>
+    <t>Filtering Sensitive Logs</t>
+  </si>
+  <si>
+    <t>config.filter_parameters += [:password] in config/application.rb (or any other symbols)</t>
+  </si>
+  <si>
+    <t>Refactoring User Name Part 1</t>
+  </si>
+  <si>
+    <t>Move view logic to models (e.g. User#full_name) when repetition occurs.</t>
+  </si>
+  <si>
+    <t>Refactoring User Name Part 2</t>
+  </si>
+  <si>
+    <t>Build tests prior to refactoring in order to ensure methods behave the same.</t>
+  </si>
+  <si>
+    <t>Refactoring User Name Part 3</t>
+  </si>
+  <si>
+    <t>Refactor tests and write methods to make model creation and method calling easier.</t>
   </si>
 </sst>
 </file>
@@ -776,8 +800,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -808,13 +838,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1147,10 +1183,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1294,20 +1330,56 @@
       <c r="B11" s="1">
         <v>9</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="4">
+        <v>41979</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1">
         <v>10</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="4">
+        <v>41979</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1">
         <v>11</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" s="4">
+        <v>41979</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="1">
         <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="4">
+        <v>41979</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 013.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="245">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -752,6 +752,12 @@
   </si>
   <si>
     <t>Refactor tests and write methods to make model creation and method calling easier.</t>
+  </si>
+  <si>
+    <t>Dangers of Model in Session</t>
+  </si>
+  <si>
+    <t>Do not store complex objects (e.g. AR models) in session varialbes as DB is not used.</t>
   </si>
 </sst>
 </file>
@@ -783,12 +789,24 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -800,7 +818,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -814,8 +832,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -837,20 +859,30 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1186,7 +1218,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1215,7 +1247,7 @@
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1229,7 +1261,7 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1243,7 +1275,7 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1257,7 +1289,7 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1271,7 +1303,7 @@
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1285,7 +1317,7 @@
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="1">
+      <c r="B8" s="8">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1299,7 +1331,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="1">
+      <c r="B9" s="8">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1313,7 +1345,7 @@
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="1">
+      <c r="B10" s="8">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1327,7 +1359,7 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="1">
+      <c r="B11" s="8">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1341,7 +1373,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="1">
+      <c r="B12" s="8">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1355,7 +1387,7 @@
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1369,7 +1401,7 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="1">
+      <c r="B14" s="8">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1383,1132 +1415,1141 @@
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="1">
+      <c r="B15" s="8">
         <v>13</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="4">
+        <v>41980</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="1">
+      <c r="B16" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="1">
+      <c r="B17" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="1">
+      <c r="B18" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="1">
+      <c r="B19" s="7">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="1">
+      <c r="B20" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="1">
+      <c r="B21" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="1">
+      <c r="B22" s="7">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="1">
+      <c r="B23" s="7">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="1">
+      <c r="B24" s="7">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="1">
+      <c r="B25" s="7">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="1">
+      <c r="B26" s="7">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="1">
+      <c r="B27" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="1">
+      <c r="B28" s="7">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="1">
+      <c r="B29" s="7">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="1">
+      <c r="B30" s="7">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="1">
+      <c r="B31" s="7">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="1">
+      <c r="B32" s="7">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="1">
+      <c r="B33" s="7">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="1">
+      <c r="B34" s="7">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="1">
+      <c r="B35" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="1">
+      <c r="B36" s="7">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="1">
+      <c r="B37" s="7">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="1">
+      <c r="B38" s="7">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="1">
+      <c r="B39" s="7">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="1">
+      <c r="B40" s="7">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="1">
+      <c r="B41" s="7">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="1">
+      <c r="B42" s="7">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="1">
+      <c r="B43" s="7">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="1">
+      <c r="B44" s="7">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="1">
+      <c r="B45" s="7">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="1">
+      <c r="B46" s="7">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="1">
+      <c r="B47" s="7">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="1">
+      <c r="B48" s="7">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="1">
+      <c r="B49" s="7">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="1">
+      <c r="B50" s="7">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="1">
+      <c r="B51" s="7">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="1">
+      <c r="B52" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="1">
+      <c r="B53" s="7">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="1">
+      <c r="B54" s="7">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="1">
+      <c r="B55" s="7">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="1">
+      <c r="B56" s="7">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="1">
+      <c r="B57" s="7">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="1">
+      <c r="B58" s="7">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="1">
+      <c r="B59" s="7">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="1">
+      <c r="B60" s="7">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="1">
+      <c r="B61" s="7">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="1">
+      <c r="B62" s="7">
         <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="1">
+      <c r="B63" s="7">
         <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="1">
+      <c r="B64" s="7">
         <v>62</v>
       </c>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="1">
+      <c r="B65" s="7">
         <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="1">
+      <c r="B66" s="7">
         <v>64</v>
       </c>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="1">
+      <c r="B67" s="7">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="1">
+      <c r="B68" s="7">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="1">
+      <c r="B69" s="7">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="1">
+      <c r="B70" s="7">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="1">
+      <c r="B71" s="7">
         <v>69</v>
       </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="1">
+      <c r="B72" s="7">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="1">
+      <c r="B73" s="7">
         <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="1">
+      <c r="B74" s="7">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="1">
+      <c r="B75" s="7">
         <v>73</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="1">
+      <c r="B76" s="7">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="1">
+      <c r="B77" s="7">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="1">
+      <c r="B78" s="7">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="1">
+      <c r="B79" s="7">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="1">
+      <c r="B80" s="7">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="1">
+      <c r="B81" s="7">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="1">
+      <c r="B82" s="7">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="1">
+      <c r="B83" s="7">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="1">
+      <c r="B84" s="7">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="1">
+      <c r="B85" s="7">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="1">
+      <c r="B86" s="7">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="1">
+      <c r="B87" s="7">
         <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="1">
+      <c r="B88" s="7">
         <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="1">
+      <c r="B89" s="7">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="1">
+      <c r="B90" s="7">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="1">
+      <c r="B91" s="7">
         <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="1">
+      <c r="B92" s="7">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="1">
+      <c r="B93" s="7">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="1">
+      <c r="B94" s="7">
         <v>92</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="1">
+      <c r="B95" s="7">
         <v>93</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="1">
+      <c r="B96" s="7">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="1">
+      <c r="B97" s="7">
         <v>95</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="1">
+      <c r="B98" s="7">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="1">
+      <c r="B99" s="7">
         <v>97</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="1">
+      <c r="B100" s="7">
         <v>98</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="1">
+      <c r="B101" s="7">
         <v>99</v>
       </c>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="1">
+      <c r="B102" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="1">
+      <c r="B103" s="7">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="1">
+      <c r="B104" s="7">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="1">
+      <c r="B105" s="7">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="1">
+      <c r="B106" s="7">
         <v>104</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="1">
+      <c r="B107" s="7">
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="1">
+      <c r="B108" s="7">
         <v>106</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="1">
+      <c r="B109" s="7">
         <v>107</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="1">
+      <c r="B110" s="7">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="1">
+      <c r="B111" s="7">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="1">
+      <c r="B112" s="7">
         <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="1">
+      <c r="B113" s="7">
         <v>111</v>
       </c>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="1">
+      <c r="B114" s="7">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="1">
+      <c r="B115" s="7">
         <v>113</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="1">
+      <c r="B116" s="7">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="1">
+      <c r="B117" s="7">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="1">
+      <c r="B118" s="7">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="1">
+      <c r="B119" s="7">
         <v>117</v>
       </c>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="1">
+      <c r="B120" s="7">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="1">
+      <c r="B121" s="7">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="1">
+      <c r="B122" s="7">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="1">
+      <c r="B123" s="7">
         <v>121</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="1">
+      <c r="B124" s="7">
         <v>122</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="1">
+      <c r="B125" s="7">
         <v>123</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="1">
+      <c r="B126" s="7">
         <v>124</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="1">
+      <c r="B127" s="7">
         <v>125</v>
       </c>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="1">
+      <c r="B128" s="7">
         <v>126</v>
       </c>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="1">
+      <c r="B129" s="7">
         <v>127</v>
       </c>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="1">
+      <c r="B130" s="7">
         <v>128</v>
       </c>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="1">
+      <c r="B131" s="7">
         <v>129</v>
       </c>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="1">
+      <c r="B132" s="7">
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="1">
+      <c r="B133" s="7">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="1">
+      <c r="B134" s="7">
         <v>132</v>
       </c>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="1">
+      <c r="B135" s="7">
         <v>133</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="1">
+      <c r="B136" s="7">
         <v>134</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="1">
+      <c r="B137" s="7">
         <v>135</v>
       </c>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="1">
+      <c r="B138" s="7">
         <v>136</v>
       </c>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="1">
+      <c r="B139" s="7">
         <v>137</v>
       </c>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="1">
+      <c r="B140" s="7">
         <v>138</v>
       </c>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="1">
+      <c r="B141" s="7">
         <v>139</v>
       </c>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="1">
+      <c r="B142" s="7">
         <v>140</v>
       </c>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="1">
+      <c r="B143" s="7">
         <v>141</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="1">
+      <c r="B144" s="7">
         <v>142</v>
       </c>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="1">
+      <c r="B145" s="7">
         <v>143</v>
       </c>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="1">
+      <c r="B146" s="7">
         <v>144</v>
       </c>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="1">
+      <c r="B147" s="7">
         <v>145</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="1">
+      <c r="B148" s="7">
         <v>146</v>
       </c>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="1">
+      <c r="B149" s="7">
         <v>147</v>
       </c>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="1">
+      <c r="B150" s="7">
         <v>148</v>
       </c>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="1">
+      <c r="B151" s="7">
         <v>149</v>
       </c>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="1">
+      <c r="B152" s="7">
         <v>150</v>
       </c>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="1">
+      <c r="B153" s="7">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="1">
+      <c r="B154" s="7">
         <v>152</v>
       </c>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="1">
+      <c r="B155" s="7">
         <v>153</v>
       </c>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="1">
+      <c r="B156" s="7">
         <v>154</v>
       </c>
     </row>
     <row r="157" spans="2:2">
-      <c r="B157" s="1">
+      <c r="B157" s="7">
         <v>155</v>
       </c>
     </row>
     <row r="158" spans="2:2">
-      <c r="B158" s="1">
+      <c r="B158" s="7">
         <v>156</v>
       </c>
     </row>
     <row r="159" spans="2:2">
-      <c r="B159" s="1">
+      <c r="B159" s="7">
         <v>157</v>
       </c>
     </row>
     <row r="160" spans="2:2">
-      <c r="B160" s="1">
+      <c r="B160" s="7">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="2:2">
-      <c r="B161" s="1">
+      <c r="B161" s="7">
         <v>159</v>
       </c>
     </row>
     <row r="162" spans="2:2">
-      <c r="B162" s="1">
+      <c r="B162" s="7">
         <v>160</v>
       </c>
     </row>
     <row r="163" spans="2:2">
-      <c r="B163" s="1">
+      <c r="B163" s="7">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="1">
+      <c r="B164" s="7">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="2:2">
-      <c r="B165" s="1">
+      <c r="B165" s="7">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="2:2">
-      <c r="B166" s="1">
+      <c r="B166" s="7">
         <v>164</v>
       </c>
     </row>
     <row r="167" spans="2:2">
-      <c r="B167" s="1">
+      <c r="B167" s="7">
         <v>165</v>
       </c>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="1">
+      <c r="B168" s="7">
         <v>166</v>
       </c>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="1">
+      <c r="B169" s="7">
         <v>167</v>
       </c>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="1">
+      <c r="B170" s="7">
         <v>168</v>
       </c>
     </row>
     <row r="171" spans="2:2">
-      <c r="B171" s="1">
+      <c r="B171" s="7">
         <v>169</v>
       </c>
     </row>
     <row r="172" spans="2:2">
-      <c r="B172" s="1">
+      <c r="B172" s="7">
         <v>170</v>
       </c>
     </row>
     <row r="173" spans="2:2">
-      <c r="B173" s="1">
+      <c r="B173" s="7">
         <v>171</v>
       </c>
     </row>
     <row r="174" spans="2:2">
-      <c r="B174" s="1">
+      <c r="B174" s="7">
         <v>172</v>
       </c>
     </row>
     <row r="175" spans="2:2">
-      <c r="B175" s="1">
+      <c r="B175" s="7">
         <v>173</v>
       </c>
     </row>
     <row r="176" spans="2:2">
-      <c r="B176" s="1">
+      <c r="B176" s="7">
         <v>174</v>
       </c>
     </row>
     <row r="177" spans="2:2">
-      <c r="B177" s="1">
+      <c r="B177" s="7">
         <v>175</v>
       </c>
     </row>
     <row r="178" spans="2:2">
-      <c r="B178" s="1">
+      <c r="B178" s="7">
         <v>176</v>
       </c>
     </row>
     <row r="179" spans="2:2">
-      <c r="B179" s="1">
+      <c r="B179" s="7">
         <v>177</v>
       </c>
     </row>
     <row r="180" spans="2:2">
-      <c r="B180" s="1">
+      <c r="B180" s="7">
         <v>178</v>
       </c>
     </row>
     <row r="181" spans="2:2">
-      <c r="B181" s="1">
+      <c r="B181" s="7">
         <v>179</v>
       </c>
     </row>
     <row r="182" spans="2:2">
-      <c r="B182" s="1">
+      <c r="B182" s="7">
         <v>180</v>
       </c>
     </row>
     <row r="183" spans="2:2">
-      <c r="B183" s="1">
+      <c r="B183" s="7">
         <v>181</v>
       </c>
     </row>
     <row r="184" spans="2:2">
-      <c r="B184" s="1">
+      <c r="B184" s="7">
         <v>182</v>
       </c>
     </row>
     <row r="185" spans="2:2">
-      <c r="B185" s="1">
+      <c r="B185" s="7">
         <v>183</v>
       </c>
     </row>
     <row r="186" spans="2:2">
-      <c r="B186" s="1">
+      <c r="B186" s="7">
         <v>184</v>
       </c>
     </row>
     <row r="187" spans="2:2">
-      <c r="B187" s="1">
+      <c r="B187" s="7">
         <v>185</v>
       </c>
     </row>
     <row r="188" spans="2:2">
-      <c r="B188" s="1">
+      <c r="B188" s="7">
         <v>186</v>
       </c>
     </row>
     <row r="189" spans="2:2">
-      <c r="B189" s="1">
+      <c r="B189" s="7">
         <v>187</v>
       </c>
     </row>
     <row r="190" spans="2:2">
-      <c r="B190" s="1">
+      <c r="B190" s="7">
         <v>188</v>
       </c>
     </row>
     <row r="191" spans="2:2">
-      <c r="B191" s="1">
+      <c r="B191" s="7">
         <v>189</v>
       </c>
     </row>
     <row r="192" spans="2:2">
-      <c r="B192" s="1">
+      <c r="B192" s="7">
         <v>190</v>
       </c>
     </row>
     <row r="193" spans="2:2">
-      <c r="B193" s="1">
+      <c r="B193" s="7">
         <v>191</v>
       </c>
     </row>
     <row r="194" spans="2:2">
-      <c r="B194" s="1">
+      <c r="B194" s="7">
         <v>192</v>
       </c>
     </row>
     <row r="195" spans="2:2">
-      <c r="B195" s="1">
+      <c r="B195" s="7">
         <v>193</v>
       </c>
     </row>
     <row r="196" spans="2:2">
-      <c r="B196" s="1">
+      <c r="B196" s="7">
         <v>194</v>
       </c>
     </row>
     <row r="197" spans="2:2">
-      <c r="B197" s="1">
+      <c r="B197" s="7">
         <v>195</v>
       </c>
     </row>
     <row r="198" spans="2:2">
-      <c r="B198" s="1">
+      <c r="B198" s="7">
         <v>196</v>
       </c>
     </row>
     <row r="199" spans="2:2">
-      <c r="B199" s="1">
+      <c r="B199" s="7">
         <v>197</v>
       </c>
     </row>
     <row r="200" spans="2:2">
-      <c r="B200" s="1">
+      <c r="B200" s="7">
         <v>198</v>
       </c>
     </row>
     <row r="201" spans="2:2">
-      <c r="B201" s="1">
+      <c r="B201" s="7">
         <v>199</v>
       </c>
     </row>
     <row r="202" spans="2:2">
-      <c r="B202" s="1">
+      <c r="B202" s="7">
         <v>200</v>
       </c>
     </row>
     <row r="203" spans="2:2">
-      <c r="B203" s="1">
+      <c r="B203" s="7">
         <v>201</v>
       </c>
     </row>
     <row r="204" spans="2:2">
-      <c r="B204" s="1">
+      <c r="B204" s="7">
         <v>202</v>
       </c>
     </row>
     <row r="205" spans="2:2">
-      <c r="B205" s="1">
+      <c r="B205" s="7">
         <v>203</v>
       </c>
     </row>
     <row r="206" spans="2:2">
-      <c r="B206" s="1">
+      <c r="B206" s="7">
         <v>204</v>
       </c>
     </row>
     <row r="207" spans="2:2">
-      <c r="B207" s="1">
+      <c r="B207" s="7">
         <v>205</v>
       </c>
     </row>
     <row r="208" spans="2:2">
-      <c r="B208" s="1">
+      <c r="B208" s="7">
         <v>206</v>
       </c>
     </row>
     <row r="209" spans="2:2">
-      <c r="B209" s="1">
+      <c r="B209" s="7">
         <v>207</v>
       </c>
     </row>
     <row r="210" spans="2:2">
-      <c r="B210" s="1">
+      <c r="B210" s="7">
         <v>208</v>
       </c>
     </row>
     <row r="211" spans="2:2">
-      <c r="B211" s="1">
+      <c r="B211" s="7">
         <v>209</v>
       </c>
     </row>
     <row r="212" spans="2:2">
-      <c r="B212" s="1">
+      <c r="B212" s="7">
         <v>210</v>
       </c>
     </row>
     <row r="213" spans="2:2">
-      <c r="B213" s="1">
+      <c r="B213" s="7">
         <v>211</v>
       </c>
     </row>
     <row r="214" spans="2:2">
-      <c r="B214" s="1">
+      <c r="B214" s="7">
         <v>212</v>
       </c>
     </row>
     <row r="215" spans="2:2">
-      <c r="B215" s="1">
+      <c r="B215" s="7">
         <v>213</v>
       </c>
     </row>
     <row r="216" spans="2:2">
-      <c r="B216" s="1">
+      <c r="B216" s="7">
         <v>214</v>
       </c>
     </row>
     <row r="217" spans="2:2">
-      <c r="B217" s="1">
+      <c r="B217" s="7">
         <v>215</v>
       </c>
     </row>
     <row r="218" spans="2:2">
-      <c r="B218" s="1">
+      <c r="B218" s="7">
         <v>216</v>
       </c>
     </row>
     <row r="219" spans="2:2">
-      <c r="B219" s="1">
+      <c r="B219" s="7">
         <v>217</v>
       </c>
     </row>
     <row r="220" spans="2:2">
-      <c r="B220" s="1">
+      <c r="B220" s="7">
         <v>218</v>
       </c>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="1">
+      <c r="B221" s="7">
         <v>219</v>
       </c>
     </row>
     <row r="222" spans="2:2">
-      <c r="B222" s="1">
+      <c r="B222" s="7">
         <v>220</v>
       </c>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="1">
+      <c r="B223" s="7">
         <v>221</v>
       </c>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="1">
+      <c r="B224" s="7">
         <v>222</v>
       </c>
     </row>
     <row r="225" spans="2:5">
-      <c r="B225" s="1">
+      <c r="B225" s="7">
         <v>223</v>
       </c>
     </row>
     <row r="226" spans="2:5">
-      <c r="B226" s="1">
+      <c r="B226" s="7">
         <v>224</v>
       </c>
     </row>
     <row r="227" spans="2:5">
-      <c r="B227" s="1">
+      <c r="B227" s="7">
         <v>225</v>
       </c>
     </row>
     <row r="228" spans="2:5">
-      <c r="B228" s="1">
+      <c r="B228" s="7">
         <v>226</v>
       </c>
     </row>
     <row r="229" spans="2:5">
-      <c r="B229" s="1">
+      <c r="B229" s="7">
         <v>227</v>
       </c>
     </row>
     <row r="230" spans="2:5">
-      <c r="B230" s="1">
+      <c r="B230" s="7">
         <v>228</v>
       </c>
     </row>
     <row r="231" spans="2:5">
-      <c r="B231" s="1">
+      <c r="B231" s="7">
         <v>229</v>
       </c>
     </row>
     <row r="232" spans="2:5">
-      <c r="B232" s="1">
+      <c r="B232" s="7">
         <v>230</v>
       </c>
     </row>
     <row r="233" spans="2:5">
-      <c r="B233" s="1">
+      <c r="B233" s="7">
         <v>231</v>
       </c>
     </row>
     <row r="234" spans="2:5">
-      <c r="B234" s="1">
+      <c r="B234" s="7">
         <v>232</v>
       </c>
     </row>
     <row r="235" spans="2:5">
-      <c r="B235" s="1">
+      <c r="B235" s="7">
         <v>233</v>
       </c>
     </row>
     <row r="236" spans="2:5">
-      <c r="B236" s="1">
+      <c r="B236" s="7">
         <v>234</v>
       </c>
     </row>
     <row r="237" spans="2:5">
-      <c r="B237" s="1">
+      <c r="B237" s="7">
         <v>235</v>
       </c>
     </row>
     <row r="238" spans="2:5">
-      <c r="B238" s="1">
+      <c r="B238" s="7">
         <v>236</v>
       </c>
     </row>
     <row r="239" spans="2:5">
-      <c r="B239" s="1">
+      <c r="B239" s="7">
         <v>237</v>
       </c>
     </row>
     <row r="240" spans="2:5">
-      <c r="B240" s="1">
+      <c r="B240" s="8">
         <v>238</v>
       </c>
       <c r="C240" s="1" t="s">
@@ -2522,187 +2563,187 @@
       </c>
     </row>
     <row r="241" spans="2:2">
-      <c r="B241" s="1">
+      <c r="B241" s="7">
         <v>239</v>
       </c>
     </row>
     <row r="242" spans="2:2">
-      <c r="B242" s="1">
+      <c r="B242" s="7">
         <v>240</v>
       </c>
     </row>
     <row r="243" spans="2:2">
-      <c r="B243" s="1">
+      <c r="B243" s="7">
         <v>241</v>
       </c>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="1">
+      <c r="B244" s="7">
         <v>242</v>
       </c>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="1">
+      <c r="B245" s="7">
         <v>243</v>
       </c>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="1">
+      <c r="B246" s="7">
         <v>244</v>
       </c>
     </row>
     <row r="247" spans="2:2">
-      <c r="B247" s="1">
+      <c r="B247" s="7">
         <v>245</v>
       </c>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="1">
+      <c r="B248" s="7">
         <v>246</v>
       </c>
     </row>
     <row r="249" spans="2:2">
-      <c r="B249" s="1">
+      <c r="B249" s="7">
         <v>247</v>
       </c>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="1">
+      <c r="B250" s="7">
         <v>248</v>
       </c>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="1">
+      <c r="B251" s="7">
         <v>249</v>
       </c>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="1">
+      <c r="B252" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="253" spans="2:2">
-      <c r="B253" s="1">
+      <c r="B253" s="7">
         <v>251</v>
       </c>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="1">
+      <c r="B254" s="7">
         <v>252</v>
       </c>
     </row>
     <row r="255" spans="2:2">
-      <c r="B255" s="1">
+      <c r="B255" s="7">
         <v>253</v>
       </c>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="1">
+      <c r="B256" s="7">
         <v>254</v>
       </c>
     </row>
     <row r="257" spans="2:2">
-      <c r="B257" s="1">
+      <c r="B257" s="7">
         <v>255</v>
       </c>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="1">
+      <c r="B258" s="7">
         <v>256</v>
       </c>
     </row>
     <row r="259" spans="2:2">
-      <c r="B259" s="1">
+      <c r="B259" s="7">
         <v>257</v>
       </c>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="1">
+      <c r="B260" s="7">
         <v>258</v>
       </c>
     </row>
     <row r="261" spans="2:2">
-      <c r="B261" s="1">
+      <c r="B261" s="7">
         <v>259</v>
       </c>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="1">
+      <c r="B262" s="7">
         <v>260</v>
       </c>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="1">
+      <c r="B263" s="7">
         <v>261</v>
       </c>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="1">
+      <c r="B264" s="7">
         <v>262</v>
       </c>
     </row>
     <row r="265" spans="2:2">
-      <c r="B265" s="1">
+      <c r="B265" s="7">
         <v>263</v>
       </c>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="1">
+      <c r="B266" s="7">
         <v>264</v>
       </c>
     </row>
     <row r="267" spans="2:2">
-      <c r="B267" s="1">
+      <c r="B267" s="7">
         <v>265</v>
       </c>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="1">
+      <c r="B268" s="7">
         <v>266</v>
       </c>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="1">
+      <c r="B269" s="7">
         <v>267</v>
       </c>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="1">
+      <c r="B270" s="7">
         <v>268</v>
       </c>
     </row>
     <row r="271" spans="2:2">
-      <c r="B271" s="1">
+      <c r="B271" s="7">
         <v>269</v>
       </c>
     </row>
     <row r="272" spans="2:2">
-      <c r="B272" s="1">
+      <c r="B272" s="7">
         <v>270</v>
       </c>
     </row>
     <row r="273" spans="2:5">
-      <c r="B273" s="1">
+      <c r="B273" s="7">
         <v>271</v>
       </c>
     </row>
     <row r="274" spans="2:5">
-      <c r="B274" s="1">
+      <c r="B274" s="7">
         <v>272</v>
       </c>
     </row>
     <row r="275" spans="2:5">
-      <c r="B275" s="1">
+      <c r="B275" s="7">
         <v>273</v>
       </c>
     </row>
     <row r="276" spans="2:5">
-      <c r="B276" s="1">
+      <c r="B276" s="7">
         <v>274</v>
       </c>
     </row>
     <row r="277" spans="2:5">
-      <c r="B277" s="1">
+      <c r="B277" s="8">
         <v>275</v>
       </c>
       <c r="C277" s="1" t="s">
@@ -2716,227 +2757,227 @@
       </c>
     </row>
     <row r="278" spans="2:5">
-      <c r="B278" s="1">
+      <c r="B278" s="7">
         <v>276</v>
       </c>
     </row>
     <row r="279" spans="2:5">
-      <c r="B279" s="1">
+      <c r="B279" s="7">
         <v>277</v>
       </c>
     </row>
     <row r="280" spans="2:5">
-      <c r="B280" s="1">
+      <c r="B280" s="7">
         <v>278</v>
       </c>
     </row>
     <row r="281" spans="2:5">
-      <c r="B281" s="1">
+      <c r="B281" s="7">
         <v>279</v>
       </c>
     </row>
     <row r="282" spans="2:5">
-      <c r="B282" s="1">
+      <c r="B282" s="7">
         <v>280</v>
       </c>
     </row>
     <row r="283" spans="2:5">
-      <c r="B283" s="1">
+      <c r="B283" s="7">
         <v>281</v>
       </c>
     </row>
     <row r="284" spans="2:5">
-      <c r="B284" s="1">
+      <c r="B284" s="7">
         <v>282</v>
       </c>
     </row>
     <row r="285" spans="2:5">
-      <c r="B285" s="1">
+      <c r="B285" s="7">
         <v>283</v>
       </c>
     </row>
     <row r="286" spans="2:5">
-      <c r="B286" s="1">
+      <c r="B286" s="7">
         <v>284</v>
       </c>
     </row>
     <row r="287" spans="2:5">
-      <c r="B287" s="1">
+      <c r="B287" s="7">
         <v>285</v>
       </c>
     </row>
     <row r="288" spans="2:5">
-      <c r="B288" s="1">
+      <c r="B288" s="7">
         <v>286</v>
       </c>
     </row>
     <row r="289" spans="2:2">
-      <c r="B289" s="1">
+      <c r="B289" s="7">
         <v>287</v>
       </c>
     </row>
     <row r="290" spans="2:2">
-      <c r="B290" s="1">
+      <c r="B290" s="7">
         <v>288</v>
       </c>
     </row>
     <row r="291" spans="2:2">
-      <c r="B291" s="1">
+      <c r="B291" s="7">
         <v>289</v>
       </c>
     </row>
     <row r="292" spans="2:2">
-      <c r="B292" s="1">
+      <c r="B292" s="7">
         <v>290</v>
       </c>
     </row>
     <row r="293" spans="2:2">
-      <c r="B293" s="1">
+      <c r="B293" s="7">
         <v>291</v>
       </c>
     </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="1">
+      <c r="B294" s="7">
         <v>292</v>
       </c>
     </row>
     <row r="295" spans="2:2">
-      <c r="B295" s="1">
+      <c r="B295" s="7">
         <v>293</v>
       </c>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="1">
+      <c r="B296" s="7">
         <v>294</v>
       </c>
     </row>
     <row r="297" spans="2:2">
-      <c r="B297" s="1">
+      <c r="B297" s="7">
         <v>295</v>
       </c>
     </row>
     <row r="298" spans="2:2">
-      <c r="B298" s="1">
+      <c r="B298" s="7">
         <v>296</v>
       </c>
     </row>
     <row r="299" spans="2:2">
-      <c r="B299" s="1">
+      <c r="B299" s="7">
         <v>297</v>
       </c>
     </row>
     <row r="300" spans="2:2">
-      <c r="B300" s="1">
+      <c r="B300" s="7">
         <v>298</v>
       </c>
     </row>
     <row r="301" spans="2:2">
-      <c r="B301" s="1">
+      <c r="B301" s="7">
         <v>299</v>
       </c>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="1">
+      <c r="B302" s="7">
         <v>300</v>
       </c>
     </row>
     <row r="303" spans="2:2">
-      <c r="B303" s="1">
+      <c r="B303" s="7">
         <v>301</v>
       </c>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="1">
+      <c r="B304" s="7">
         <v>302</v>
       </c>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="1">
+      <c r="B305" s="7">
         <v>303</v>
       </c>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="1">
+      <c r="B306" s="7">
         <v>304</v>
       </c>
     </row>
     <row r="307" spans="2:2">
-      <c r="B307" s="1">
+      <c r="B307" s="7">
         <v>305</v>
       </c>
     </row>
     <row r="308" spans="2:2">
-      <c r="B308" s="1">
+      <c r="B308" s="7">
         <v>306</v>
       </c>
     </row>
     <row r="309" spans="2:2">
-      <c r="B309" s="1">
+      <c r="B309" s="7">
         <v>307</v>
       </c>
     </row>
     <row r="310" spans="2:2">
-      <c r="B310" s="1">
+      <c r="B310" s="7">
         <v>308</v>
       </c>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="1">
+      <c r="B311" s="7">
         <v>309</v>
       </c>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="1">
+      <c r="B312" s="7">
         <v>310</v>
       </c>
     </row>
     <row r="313" spans="2:2">
-      <c r="B313" s="1">
+      <c r="B313" s="7">
         <v>311</v>
       </c>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="1">
+      <c r="B314" s="7">
         <v>312</v>
       </c>
     </row>
     <row r="315" spans="2:2">
-      <c r="B315" s="1">
+      <c r="B315" s="7">
         <v>313</v>
       </c>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="1">
+      <c r="B316" s="7">
         <v>314</v>
       </c>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="1">
+      <c r="B317" s="7">
         <v>315</v>
       </c>
     </row>
     <row r="318" spans="2:2">
-      <c r="B318" s="1">
+      <c r="B318" s="7">
         <v>316</v>
       </c>
     </row>
     <row r="319" spans="2:2">
-      <c r="B319" s="1">
+      <c r="B319" s="7">
         <v>317</v>
       </c>
     </row>
     <row r="320" spans="2:2">
-      <c r="B320" s="1">
+      <c r="B320" s="7">
         <v>318</v>
       </c>
     </row>
     <row r="321" spans="2:5">
-      <c r="B321" s="1">
+      <c r="B321" s="7">
         <v>319</v>
       </c>
     </row>
     <row r="322" spans="2:5">
-      <c r="B322" s="1">
+      <c r="B322" s="8">
         <v>320</v>
       </c>
       <c r="C322" s="1" t="s">
@@ -2950,487 +2991,487 @@
       </c>
     </row>
     <row r="323" spans="2:5">
-      <c r="B323" s="1">
+      <c r="B323" s="7">
         <v>321</v>
       </c>
     </row>
     <row r="324" spans="2:5">
-      <c r="B324" s="1">
+      <c r="B324" s="7">
         <v>322</v>
       </c>
     </row>
     <row r="325" spans="2:5">
-      <c r="B325" s="1">
+      <c r="B325" s="7">
         <v>323</v>
       </c>
     </row>
     <row r="326" spans="2:5">
-      <c r="B326" s="1">
+      <c r="B326" s="7">
         <v>324</v>
       </c>
     </row>
     <row r="327" spans="2:5">
-      <c r="B327" s="1">
+      <c r="B327" s="7">
         <v>325</v>
       </c>
     </row>
     <row r="328" spans="2:5">
-      <c r="B328" s="1">
+      <c r="B328" s="7">
         <v>326</v>
       </c>
     </row>
     <row r="329" spans="2:5">
-      <c r="B329" s="1">
+      <c r="B329" s="7">
         <v>327</v>
       </c>
     </row>
     <row r="330" spans="2:5">
-      <c r="B330" s="1">
+      <c r="B330" s="7">
         <v>328</v>
       </c>
     </row>
     <row r="331" spans="2:5">
-      <c r="B331" s="1">
+      <c r="B331" s="7">
         <v>329</v>
       </c>
     </row>
     <row r="332" spans="2:5">
-      <c r="B332" s="1">
+      <c r="B332" s="7">
         <v>330</v>
       </c>
     </row>
     <row r="333" spans="2:5">
-      <c r="B333" s="1">
+      <c r="B333" s="7">
         <v>331</v>
       </c>
     </row>
     <row r="334" spans="2:5">
-      <c r="B334" s="1">
+      <c r="B334" s="7">
         <v>332</v>
       </c>
     </row>
     <row r="335" spans="2:5">
-      <c r="B335" s="1">
+      <c r="B335" s="7">
         <v>333</v>
       </c>
     </row>
     <row r="336" spans="2:5">
-      <c r="B336" s="1">
+      <c r="B336" s="7">
         <v>334</v>
       </c>
     </row>
     <row r="337" spans="2:2">
-      <c r="B337" s="1">
+      <c r="B337" s="7">
         <v>335</v>
       </c>
     </row>
     <row r="338" spans="2:2">
-      <c r="B338" s="1">
+      <c r="B338" s="7">
         <v>336</v>
       </c>
     </row>
     <row r="339" spans="2:2">
-      <c r="B339" s="1">
+      <c r="B339" s="7">
         <v>337</v>
       </c>
     </row>
     <row r="340" spans="2:2">
-      <c r="B340" s="1">
+      <c r="B340" s="7">
         <v>338</v>
       </c>
     </row>
     <row r="341" spans="2:2">
-      <c r="B341" s="1">
+      <c r="B341" s="7">
         <v>339</v>
       </c>
     </row>
     <row r="342" spans="2:2">
-      <c r="B342" s="1">
+      <c r="B342" s="7">
         <v>340</v>
       </c>
     </row>
     <row r="343" spans="2:2">
-      <c r="B343" s="1">
+      <c r="B343" s="7">
         <v>341</v>
       </c>
     </row>
     <row r="344" spans="2:2">
-      <c r="B344" s="1">
+      <c r="B344" s="7">
         <v>342</v>
       </c>
     </row>
     <row r="345" spans="2:2">
-      <c r="B345" s="1">
+      <c r="B345" s="7">
         <v>343</v>
       </c>
     </row>
     <row r="346" spans="2:2">
-      <c r="B346" s="1">
+      <c r="B346" s="7">
         <v>344</v>
       </c>
     </row>
     <row r="347" spans="2:2">
-      <c r="B347" s="1">
+      <c r="B347" s="7">
         <v>345</v>
       </c>
     </row>
     <row r="348" spans="2:2">
-      <c r="B348" s="1">
+      <c r="B348" s="7">
         <v>346</v>
       </c>
     </row>
     <row r="349" spans="2:2">
-      <c r="B349" s="1">
+      <c r="B349" s="7">
         <v>347</v>
       </c>
     </row>
     <row r="350" spans="2:2">
-      <c r="B350" s="1">
+      <c r="B350" s="7">
         <v>348</v>
       </c>
     </row>
     <row r="351" spans="2:2">
-      <c r="B351" s="1">
+      <c r="B351" s="7">
         <v>349</v>
       </c>
     </row>
     <row r="352" spans="2:2">
-      <c r="B352" s="1">
+      <c r="B352" s="7">
         <v>350</v>
       </c>
     </row>
     <row r="353" spans="2:2">
-      <c r="B353" s="1">
+      <c r="B353" s="7">
         <v>351</v>
       </c>
     </row>
     <row r="354" spans="2:2">
-      <c r="B354" s="1">
+      <c r="B354" s="7">
         <v>352</v>
       </c>
     </row>
     <row r="355" spans="2:2">
-      <c r="B355" s="1">
+      <c r="B355" s="7">
         <v>353</v>
       </c>
     </row>
     <row r="356" spans="2:2">
-      <c r="B356" s="1">
+      <c r="B356" s="7">
         <v>354</v>
       </c>
     </row>
     <row r="357" spans="2:2">
-      <c r="B357" s="1">
+      <c r="B357" s="7">
         <v>355</v>
       </c>
     </row>
     <row r="358" spans="2:2">
-      <c r="B358" s="1">
+      <c r="B358" s="7">
         <v>356</v>
       </c>
     </row>
     <row r="359" spans="2:2">
-      <c r="B359" s="1">
+      <c r="B359" s="7">
         <v>357</v>
       </c>
     </row>
     <row r="360" spans="2:2">
-      <c r="B360" s="1">
+      <c r="B360" s="7">
         <v>358</v>
       </c>
     </row>
     <row r="361" spans="2:2">
-      <c r="B361" s="1">
+      <c r="B361" s="7">
         <v>359</v>
       </c>
     </row>
     <row r="362" spans="2:2">
-      <c r="B362" s="1">
+      <c r="B362" s="7">
         <v>360</v>
       </c>
     </row>
     <row r="363" spans="2:2">
-      <c r="B363" s="1">
+      <c r="B363" s="7">
         <v>361</v>
       </c>
     </row>
     <row r="364" spans="2:2">
-      <c r="B364" s="1">
+      <c r="B364" s="7">
         <v>362</v>
       </c>
     </row>
     <row r="365" spans="2:2">
-      <c r="B365" s="1">
+      <c r="B365" s="7">
         <v>363</v>
       </c>
     </row>
     <row r="366" spans="2:2">
-      <c r="B366" s="1">
+      <c r="B366" s="7">
         <v>364</v>
       </c>
     </row>
     <row r="367" spans="2:2">
-      <c r="B367" s="1">
+      <c r="B367" s="7">
         <v>365</v>
       </c>
     </row>
     <row r="368" spans="2:2">
-      <c r="B368" s="1">
+      <c r="B368" s="7">
         <v>366</v>
       </c>
     </row>
     <row r="369" spans="2:2">
-      <c r="B369" s="1">
+      <c r="B369" s="7">
         <v>367</v>
       </c>
     </row>
     <row r="370" spans="2:2">
-      <c r="B370" s="1">
+      <c r="B370" s="7">
         <v>368</v>
       </c>
     </row>
     <row r="371" spans="2:2">
-      <c r="B371" s="1">
+      <c r="B371" s="7">
         <v>369</v>
       </c>
     </row>
     <row r="372" spans="2:2">
-      <c r="B372" s="1">
+      <c r="B372" s="7">
         <v>370</v>
       </c>
     </row>
     <row r="373" spans="2:2">
-      <c r="B373" s="1">
+      <c r="B373" s="7">
         <v>371</v>
       </c>
     </row>
     <row r="374" spans="2:2">
-      <c r="B374" s="1">
+      <c r="B374" s="7">
         <v>372</v>
       </c>
     </row>
     <row r="375" spans="2:2">
-      <c r="B375" s="1">
+      <c r="B375" s="7">
         <v>373</v>
       </c>
     </row>
     <row r="376" spans="2:2">
-      <c r="B376" s="1">
+      <c r="B376" s="7">
         <v>374</v>
       </c>
     </row>
     <row r="377" spans="2:2">
-      <c r="B377" s="1">
+      <c r="B377" s="7">
         <v>375</v>
       </c>
     </row>
     <row r="378" spans="2:2">
-      <c r="B378" s="1">
+      <c r="B378" s="7">
         <v>376</v>
       </c>
     </row>
     <row r="379" spans="2:2">
-      <c r="B379" s="1">
+      <c r="B379" s="7">
         <v>377</v>
       </c>
     </row>
     <row r="380" spans="2:2">
-      <c r="B380" s="1">
+      <c r="B380" s="7">
         <v>378</v>
       </c>
     </row>
     <row r="381" spans="2:2">
-      <c r="B381" s="1">
+      <c r="B381" s="7">
         <v>379</v>
       </c>
     </row>
     <row r="382" spans="2:2">
-      <c r="B382" s="1">
+      <c r="B382" s="7">
         <v>380</v>
       </c>
     </row>
     <row r="383" spans="2:2">
-      <c r="B383" s="1">
+      <c r="B383" s="7">
         <v>381</v>
       </c>
     </row>
     <row r="384" spans="2:2">
-      <c r="B384" s="1">
+      <c r="B384" s="7">
         <v>382</v>
       </c>
     </row>
     <row r="385" spans="2:2">
-      <c r="B385" s="1">
+      <c r="B385" s="7">
         <v>383</v>
       </c>
     </row>
     <row r="386" spans="2:2">
-      <c r="B386" s="1">
+      <c r="B386" s="7">
         <v>384</v>
       </c>
     </row>
     <row r="387" spans="2:2">
-      <c r="B387" s="1">
+      <c r="B387" s="7">
         <v>385</v>
       </c>
     </row>
     <row r="388" spans="2:2">
-      <c r="B388" s="1">
+      <c r="B388" s="7">
         <v>386</v>
       </c>
     </row>
     <row r="389" spans="2:2">
-      <c r="B389" s="1">
+      <c r="B389" s="7">
         <v>387</v>
       </c>
     </row>
     <row r="390" spans="2:2">
-      <c r="B390" s="1">
+      <c r="B390" s="7">
         <v>388</v>
       </c>
     </row>
     <row r="391" spans="2:2">
-      <c r="B391" s="1">
+      <c r="B391" s="7">
         <v>389</v>
       </c>
     </row>
     <row r="392" spans="2:2">
-      <c r="B392" s="1">
+      <c r="B392" s="7">
         <v>390</v>
       </c>
     </row>
     <row r="393" spans="2:2">
-      <c r="B393" s="1">
+      <c r="B393" s="7">
         <v>391</v>
       </c>
     </row>
     <row r="394" spans="2:2">
-      <c r="B394" s="1">
+      <c r="B394" s="7">
         <v>392</v>
       </c>
     </row>
     <row r="395" spans="2:2">
-      <c r="B395" s="1">
+      <c r="B395" s="7">
         <v>393</v>
       </c>
     </row>
     <row r="396" spans="2:2">
-      <c r="B396" s="1">
+      <c r="B396" s="7">
         <v>394</v>
       </c>
     </row>
     <row r="397" spans="2:2">
-      <c r="B397" s="1">
+      <c r="B397" s="7">
         <v>395</v>
       </c>
     </row>
     <row r="398" spans="2:2">
-      <c r="B398" s="1">
+      <c r="B398" s="7">
         <v>396</v>
       </c>
     </row>
     <row r="399" spans="2:2">
-      <c r="B399" s="1">
+      <c r="B399" s="7">
         <v>397</v>
       </c>
     </row>
     <row r="400" spans="2:2">
-      <c r="B400" s="1">
+      <c r="B400" s="7">
         <v>398</v>
       </c>
     </row>
     <row r="401" spans="2:2">
-      <c r="B401" s="1">
+      <c r="B401" s="7">
         <v>399</v>
       </c>
     </row>
     <row r="402" spans="2:2">
-      <c r="B402" s="1">
+      <c r="B402" s="7">
         <v>400</v>
       </c>
     </row>
     <row r="403" spans="2:2">
-      <c r="B403" s="1">
+      <c r="B403" s="7">
         <v>401</v>
       </c>
     </row>
     <row r="404" spans="2:2">
-      <c r="B404" s="1">
+      <c r="B404" s="7">
         <v>402</v>
       </c>
     </row>
     <row r="405" spans="2:2">
-      <c r="B405" s="1">
+      <c r="B405" s="7">
         <v>403</v>
       </c>
     </row>
     <row r="406" spans="2:2">
-      <c r="B406" s="1">
+      <c r="B406" s="7">
         <v>404</v>
       </c>
     </row>
     <row r="407" spans="2:2">
-      <c r="B407" s="1">
+      <c r="B407" s="7">
         <v>405</v>
       </c>
     </row>
     <row r="408" spans="2:2">
-      <c r="B408" s="1">
+      <c r="B408" s="7">
         <v>406</v>
       </c>
     </row>
     <row r="409" spans="2:2">
-      <c r="B409" s="1">
+      <c r="B409" s="7">
         <v>407</v>
       </c>
     </row>
     <row r="410" spans="2:2">
-      <c r="B410" s="1">
+      <c r="B410" s="7">
         <v>408</v>
       </c>
     </row>
     <row r="411" spans="2:2">
-      <c r="B411" s="1">
+      <c r="B411" s="7">
         <v>409</v>
       </c>
     </row>
     <row r="412" spans="2:2">
-      <c r="B412" s="1">
+      <c r="B412" s="7">
         <v>410</v>
       </c>
     </row>
     <row r="413" spans="2:2">
-      <c r="B413" s="1">
+      <c r="B413" s="7">
         <v>411</v>
       </c>
     </row>
     <row r="414" spans="2:2">
-      <c r="B414" s="1">
+      <c r="B414" s="7">
         <v>412</v>
       </c>
     </row>
     <row r="415" spans="2:2">
-      <c r="B415" s="1">
+      <c r="B415" s="7">
         <v>413</v>
       </c>
     </row>
     <row r="416" spans="2:2">
-      <c r="B416" s="1">
+      <c r="B416" s="7">
         <v>414</v>
       </c>
     </row>
     <row r="417" spans="2:2">
-      <c r="B417" s="1">
+      <c r="B417" s="7">
         <v>415</v>
       </c>
     </row>
     <row r="418" spans="2:2">
-      <c r="B418" s="1">
+      <c r="B418" s="7">
         <v>416</v>
       </c>
     </row>
     <row r="419" spans="2:2">
-      <c r="B419" s="1">
+      <c r="B419" s="7">
         <v>417</v>
       </c>
     </row>
@@ -3454,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 014.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="247">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -758,6 +758,12 @@
   </si>
   <si>
     <t>Do not store complex objects (e.g. AR models) in session varialbes as DB is not used.</t>
+  </si>
+  <si>
+    <t>Performing Calculations on Models</t>
+  </si>
+  <si>
+    <t>Use methods like .average, .minimum, .maximum, and .sum on AR models and associations.</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1224,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1429,8 +1435,17 @@
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="7">
+      <c r="B16" s="8">
         <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D16" s="4">
+        <v>41982</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:2">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 015.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="249">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -764,6 +764,12 @@
   </si>
   <si>
     <t>Use methods like .average, .minimum, .maximum, and .sum on AR models and associations.</t>
+  </si>
+  <si>
+    <t>Fun with Find Conditions</t>
+  </si>
+  <si>
+    <t>Can pass in arrays, ranges, and nil values to find [ e.g. Task.find_by_priority(1..5) ].</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1230,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1448,82 +1454,91 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="7">
+    <row r="17" spans="2:5">
+      <c r="B17" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:2">
+      <c r="C17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="4">
+        <v>41983</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:5">
       <c r="B19" s="7">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:5">
       <c r="B20" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:5">
       <c r="B21" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:5">
       <c r="B22" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:5">
       <c r="B23" s="7">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:5">
       <c r="B24" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:5">
       <c r="B25" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:5">
       <c r="B26" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:5">
       <c r="B27" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:5">
       <c r="B28" s="7">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="2:5">
       <c r="B29" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:5">
       <c r="B30" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:5">
       <c r="B31" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="2:5">
       <c r="B32" s="7">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 016.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="251">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -770,6 +770,12 @@
   </si>
   <si>
     <t>Can pass in arrays, ranges, and nil values to find [ e.g. Task.find_by_priority(1..5) ].</t>
+  </si>
+  <si>
+    <t>Virtual Attributes</t>
+  </si>
+  <si>
+    <t>Virtual attributes can be used to improve UI w/o impacting storage in database.</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1236,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1469,8 +1475,17 @@
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="7">
+      <c r="B18" s="8">
         <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" s="4">
+        <v>41984</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 017.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="253">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -776,6 +776,12 @@
   </si>
   <si>
     <t>Virtual attributes can be used to improve UI w/o impacting storage in database.</t>
+  </si>
+  <si>
+    <t>HABTM Checkboxes</t>
+  </si>
+  <si>
+    <t>Build HABTM checkboxes to change associations. * dom_id( ) and AR_ids = [ ] to set relationships. *</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1242,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1489,8 +1495,17 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="4">
+        <v>41986</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 018.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="255">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -782,6 +782,12 @@
   </si>
   <si>
     <t>Build HABTM checkboxes to change associations. * dom_id( ) and AR_ids = [ ] to set relationships. *</t>
+  </si>
+  <si>
+    <t>&lt;% flash.each do |key, msg| %&gt; &lt;%= content_tag :div, msg, :id =&gt; key %&gt; &lt;% end %&gt; for flash.</t>
+  </si>
+  <si>
+    <t>Looping Through Flash</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1248,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1509,8 +1515,17 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="7">
+      <c r="B20" s="8">
         <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D20" s="4">
+        <v>41987</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 019, 020, 021.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="261">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -788,6 +788,24 @@
   </si>
   <si>
     <t>Looping Through Flash</t>
+  </si>
+  <si>
+    <t>Where Administration Goes</t>
+  </si>
+  <si>
+    <t>Separation of admin/ interface isn't always necessary; recommend doing it inline on index pages.</t>
+  </si>
+  <si>
+    <t>Restricting Access</t>
+  </si>
+  <si>
+    <t>Use of admin? and before_filter :authorize, :except =&gt; :index to protect pages from being visited.</t>
+  </si>
+  <si>
+    <t>Super Simple Authentication</t>
+  </si>
+  <si>
+    <t>Use session[:password] via /login action &amp; match via admin? to allow admin access to simple site.</t>
   </si>
 </sst>
 </file>
@@ -848,8 +866,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -896,7 +918,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -905,6 +927,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -913,6 +937,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1248,7 +1274,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1529,18 +1555,45 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>19</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" s="4">
+        <v>41988</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="7">
+      <c r="B22" s="8">
         <v>20</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="4">
+        <v>41988</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="7">
+      <c r="B23" s="8">
         <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" s="4">
+        <v>41988</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 022.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="263">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -806,6 +806,12 @@
   </si>
   <si>
     <t>Use session[:password] via /login action &amp; match via admin? to allow admin access to simple site.</t>
+  </si>
+  <si>
+    <t>Eager Loading</t>
+  </si>
+  <si>
+    <t>Use eager loading to load additional model associations to reduce SQL queries run in project.</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1280,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1597,8 +1603,17 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="7">
+      <c r="B24" s="8">
         <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" s="4">
+        <v>41989</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 023.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="265">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -812,6 +812,12 @@
   </si>
   <si>
     <t>Use eager loading to load additional model associations to reduce SQL queries run in project.</t>
+  </si>
+  <si>
+    <t>Counter Cache Column</t>
+  </si>
+  <si>
+    <t>Keep track of DB model count in base model (belongs_to :base, :counter_cache =&gt; true)</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1286,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1617,8 +1623,17 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="7">
+      <c r="B25" s="8">
         <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D25" s="4">
+        <v>41990</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 024.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="1220" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="267">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -818,6 +818,12 @@
   </si>
   <si>
     <t>Keep track of DB model count in base model (belongs_to :base, :counter_cache =&gt; true)</t>
+  </si>
+  <si>
+    <t>The Stack Trace</t>
+  </si>
+  <si>
+    <t>The stack trace when in Ruby / Rails is useful in debugging precisely where issues occur.</t>
   </si>
 </sst>
 </file>
@@ -1637,8 +1643,17 @@
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="7">
+      <c r="B26" s="8">
         <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D26" s="4">
+        <v>41999</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 025.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1220" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="269">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -824,12 +824,21 @@
   </si>
   <si>
     <t>The stack trace when in Ruby / Rails is useful in debugging precisely where issues occur.</t>
+  </si>
+  <si>
+    <t>SQL Injection</t>
+  </si>
+  <si>
+    <t>Use ? to prevent SQL Injection - e.g. Model.where(["name LIKE ?", "%#{params[:query]}%"])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -907,7 +916,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -920,19 +929,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1292,7 +1304,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1300,7 +1312,7 @@
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
     <col min="5" max="5" width="75.83203125" style="3" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1313,7 +1325,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>212</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1321,13 +1333,13 @@
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="8">
         <v>41521</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1335,13 +1347,13 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="8">
         <v>41521</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1349,13 +1361,13 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="8">
         <v>41521</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1363,13 +1375,13 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="8">
+      <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="9">
         <v>41524</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1377,13 +1389,13 @@
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="9">
         <v>41557</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1391,13 +1403,13 @@
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <v>41974</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1405,13 +1417,13 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6">
         <v>41974</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1419,13 +1431,13 @@
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="6">
         <v>41975</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1433,13 +1445,13 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6">
         <v>41979</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1447,13 +1459,13 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="6">
         <v>41979</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1461,13 +1473,13 @@
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="6">
         <v>41979</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1475,13 +1487,13 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="6">
         <v>41979</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1489,13 +1501,13 @@
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="8">
+      <c r="B15" s="5">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="6">
         <v>41980</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1503,13 +1515,13 @@
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="6">
         <v>41982</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1517,13 +1529,13 @@
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="6">
         <v>41983</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1531,13 +1543,13 @@
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="8">
+      <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="6">
         <v>41984</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1545,13 +1557,13 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="8">
+      <c r="B19" s="5">
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="6">
         <v>41986</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1559,13 +1571,13 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="8">
+      <c r="B20" s="5">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="6">
         <v>41987</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1573,13 +1585,13 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="8">
+      <c r="B21" s="5">
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="6">
         <v>41988</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1587,13 +1599,13 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="8">
+      <c r="B22" s="5">
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="6">
         <v>41988</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1601,13 +1613,13 @@
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="8">
+      <c r="B23" s="5">
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="6">
         <v>41988</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1615,13 +1627,13 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="8">
+      <c r="B24" s="5">
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="6">
         <v>41989</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1629,13 +1641,13 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="8">
+      <c r="B25" s="5">
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="6">
         <v>41990</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1643,13 +1655,13 @@
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="8">
+      <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="6">
         <v>41999</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1657,1078 +1669,1087 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>25</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" s="6">
+        <v>42005</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="7">
+      <c r="B29" s="4">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="7">
+      <c r="B30" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="7">
+      <c r="B31" s="4">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="7">
+      <c r="B32" s="4">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="7">
+      <c r="B33" s="4">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="7">
+      <c r="B34" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="7">
+      <c r="B35" s="4">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="7">
+      <c r="B36" s="4">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="7">
+      <c r="B37" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="7">
+      <c r="B38" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="7">
+      <c r="B39" s="4">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="7">
+      <c r="B40" s="4">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="7">
+      <c r="B41" s="4">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="7">
+      <c r="B42" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="7">
+      <c r="B43" s="4">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="7">
+      <c r="B44" s="4">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="7">
+      <c r="B45" s="4">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="7">
+      <c r="B46" s="4">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="7">
+      <c r="B47" s="4">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="7">
+      <c r="B49" s="4">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="7">
+      <c r="B50" s="4">
         <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="7">
+      <c r="B51" s="4">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="7">
+      <c r="B52" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="7">
+      <c r="B53" s="4">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="7">
+      <c r="B54" s="4">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="7">
+      <c r="B55" s="4">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="7">
+      <c r="B56" s="4">
         <v>54</v>
       </c>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="7">
+      <c r="B57" s="4">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="7">
+      <c r="B58" s="4">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="7">
+      <c r="B59" s="4">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="7">
+      <c r="B60" s="4">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="7">
+      <c r="B61" s="4">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="7">
+      <c r="B62" s="4">
         <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="7">
+      <c r="B63" s="4">
         <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="7">
+      <c r="B64" s="4">
         <v>62</v>
       </c>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="7">
+      <c r="B65" s="4">
         <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="7">
+      <c r="B66" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="7">
+      <c r="B67" s="4">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="7">
+      <c r="B68" s="4">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="7">
+      <c r="B69" s="4">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="7">
+      <c r="B70" s="4">
         <v>68</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="7">
+      <c r="B71" s="4">
         <v>69</v>
       </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="7">
+      <c r="B72" s="4">
         <v>70</v>
       </c>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="7">
+      <c r="B73" s="4">
         <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="7">
+      <c r="B74" s="4">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="7">
+      <c r="B75" s="4">
         <v>73</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="7">
+      <c r="B76" s="4">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="7">
+      <c r="B77" s="4">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="7">
+      <c r="B78" s="4">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="7">
+      <c r="B79" s="4">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="7">
+      <c r="B80" s="4">
         <v>78</v>
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="7">
+      <c r="B81" s="4">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="7">
+      <c r="B82" s="4">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="7">
+      <c r="B83" s="4">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="7">
+      <c r="B84" s="4">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="7">
+      <c r="B85" s="4">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="7">
+      <c r="B86" s="4">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="7">
+      <c r="B87" s="4">
         <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="7">
+      <c r="B88" s="4">
         <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="7">
+      <c r="B89" s="4">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="7">
+      <c r="B90" s="4">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="7">
+      <c r="B91" s="4">
         <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="7">
+      <c r="B92" s="4">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="7">
+      <c r="B93" s="4">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="7">
+      <c r="B94" s="4">
         <v>92</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="7">
+      <c r="B95" s="4">
         <v>93</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="7">
+      <c r="B96" s="4">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="7">
+      <c r="B97" s="4">
         <v>95</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="7">
+      <c r="B98" s="4">
         <v>96</v>
       </c>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="7">
+      <c r="B99" s="4">
         <v>97</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="7">
+      <c r="B100" s="4">
         <v>98</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="7">
+      <c r="B101" s="4">
         <v>99</v>
       </c>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="7">
+      <c r="B102" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="7">
+      <c r="B103" s="4">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="7">
+      <c r="B104" s="4">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="7">
+      <c r="B105" s="4">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="7">
+      <c r="B106" s="4">
         <v>104</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="7">
+      <c r="B107" s="4">
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="7">
+      <c r="B108" s="4">
         <v>106</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="7">
+      <c r="B109" s="4">
         <v>107</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="7">
+      <c r="B110" s="4">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="7">
+      <c r="B111" s="4">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="7">
+      <c r="B112" s="4">
         <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="7">
+      <c r="B113" s="4">
         <v>111</v>
       </c>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="7">
+      <c r="B114" s="4">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="7">
+      <c r="B115" s="4">
         <v>113</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="7">
+      <c r="B116" s="4">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="7">
+      <c r="B117" s="4">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="7">
+      <c r="B118" s="4">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="7">
+      <c r="B119" s="4">
         <v>117</v>
       </c>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="7">
+      <c r="B120" s="4">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="7">
+      <c r="B121" s="4">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="7">
+      <c r="B122" s="4">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="7">
+      <c r="B123" s="4">
         <v>121</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="7">
+      <c r="B124" s="4">
         <v>122</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="7">
+      <c r="B125" s="4">
         <v>123</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="7">
+      <c r="B126" s="4">
         <v>124</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="7">
+      <c r="B127" s="4">
         <v>125</v>
       </c>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="7">
+      <c r="B128" s="4">
         <v>126</v>
       </c>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="7">
+      <c r="B129" s="4">
         <v>127</v>
       </c>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="7">
+      <c r="B130" s="4">
         <v>128</v>
       </c>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="7">
+      <c r="B131" s="4">
         <v>129</v>
       </c>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="7">
+      <c r="B132" s="4">
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="7">
+      <c r="B133" s="4">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="7">
+      <c r="B134" s="4">
         <v>132</v>
       </c>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="7">
+      <c r="B135" s="4">
         <v>133</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="7">
+      <c r="B136" s="4">
         <v>134</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="7">
+      <c r="B137" s="4">
         <v>135</v>
       </c>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="7">
+      <c r="B138" s="4">
         <v>136</v>
       </c>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="7">
+      <c r="B139" s="4">
         <v>137</v>
       </c>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="7">
+      <c r="B140" s="4">
         <v>138</v>
       </c>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="7">
+      <c r="B141" s="4">
         <v>139</v>
       </c>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="7">
+      <c r="B142" s="4">
         <v>140</v>
       </c>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="7">
+      <c r="B143" s="4">
         <v>141</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="7">
+      <c r="B144" s="4">
         <v>142</v>
       </c>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="7">
+      <c r="B145" s="4">
         <v>143</v>
       </c>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="7">
+      <c r="B146" s="4">
         <v>144</v>
       </c>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="7">
+      <c r="B147" s="4">
         <v>145</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="7">
+      <c r="B148" s="4">
         <v>146</v>
       </c>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="7">
+      <c r="B149" s="4">
         <v>147</v>
       </c>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="7">
+      <c r="B150" s="4">
         <v>148</v>
       </c>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="7">
+      <c r="B151" s="4">
         <v>149</v>
       </c>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="7">
+      <c r="B152" s="4">
         <v>150</v>
       </c>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="7">
+      <c r="B153" s="4">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="7">
+      <c r="B154" s="4">
         <v>152</v>
       </c>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="7">
+      <c r="B155" s="4">
         <v>153</v>
       </c>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="7">
+      <c r="B156" s="4">
         <v>154</v>
       </c>
     </row>
     <row r="157" spans="2:2">
-      <c r="B157" s="7">
+      <c r="B157" s="4">
         <v>155</v>
       </c>
     </row>
     <row r="158" spans="2:2">
-      <c r="B158" s="7">
+      <c r="B158" s="4">
         <v>156</v>
       </c>
     </row>
     <row r="159" spans="2:2">
-      <c r="B159" s="7">
+      <c r="B159" s="4">
         <v>157</v>
       </c>
     </row>
     <row r="160" spans="2:2">
-      <c r="B160" s="7">
+      <c r="B160" s="4">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="2:2">
-      <c r="B161" s="7">
+      <c r="B161" s="4">
         <v>159</v>
       </c>
     </row>
     <row r="162" spans="2:2">
-      <c r="B162" s="7">
+      <c r="B162" s="4">
         <v>160</v>
       </c>
     </row>
     <row r="163" spans="2:2">
-      <c r="B163" s="7">
+      <c r="B163" s="4">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="7">
+      <c r="B164" s="4">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="2:2">
-      <c r="B165" s="7">
+      <c r="B165" s="4">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="2:2">
-      <c r="B166" s="7">
+      <c r="B166" s="4">
         <v>164</v>
       </c>
     </row>
     <row r="167" spans="2:2">
-      <c r="B167" s="7">
+      <c r="B167" s="4">
         <v>165</v>
       </c>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="7">
+      <c r="B168" s="4">
         <v>166</v>
       </c>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="7">
+      <c r="B169" s="4">
         <v>167</v>
       </c>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="7">
+      <c r="B170" s="4">
         <v>168</v>
       </c>
     </row>
     <row r="171" spans="2:2">
-      <c r="B171" s="7">
+      <c r="B171" s="4">
         <v>169</v>
       </c>
     </row>
     <row r="172" spans="2:2">
-      <c r="B172" s="7">
+      <c r="B172" s="4">
         <v>170</v>
       </c>
     </row>
     <row r="173" spans="2:2">
-      <c r="B173" s="7">
+      <c r="B173" s="4">
         <v>171</v>
       </c>
     </row>
     <row r="174" spans="2:2">
-      <c r="B174" s="7">
+      <c r="B174" s="4">
         <v>172</v>
       </c>
     </row>
     <row r="175" spans="2:2">
-      <c r="B175" s="7">
+      <c r="B175" s="4">
         <v>173</v>
       </c>
     </row>
     <row r="176" spans="2:2">
-      <c r="B176" s="7">
+      <c r="B176" s="4">
         <v>174</v>
       </c>
     </row>
     <row r="177" spans="2:2">
-      <c r="B177" s="7">
+      <c r="B177" s="4">
         <v>175</v>
       </c>
     </row>
     <row r="178" spans="2:2">
-      <c r="B178" s="7">
+      <c r="B178" s="4">
         <v>176</v>
       </c>
     </row>
     <row r="179" spans="2:2">
-      <c r="B179" s="7">
+      <c r="B179" s="4">
         <v>177</v>
       </c>
     </row>
     <row r="180" spans="2:2">
-      <c r="B180" s="7">
+      <c r="B180" s="4">
         <v>178</v>
       </c>
     </row>
     <row r="181" spans="2:2">
-      <c r="B181" s="7">
+      <c r="B181" s="4">
         <v>179</v>
       </c>
     </row>
     <row r="182" spans="2:2">
-      <c r="B182" s="7">
+      <c r="B182" s="4">
         <v>180</v>
       </c>
     </row>
     <row r="183" spans="2:2">
-      <c r="B183" s="7">
+      <c r="B183" s="4">
         <v>181</v>
       </c>
     </row>
     <row r="184" spans="2:2">
-      <c r="B184" s="7">
+      <c r="B184" s="4">
         <v>182</v>
       </c>
     </row>
     <row r="185" spans="2:2">
-      <c r="B185" s="7">
+      <c r="B185" s="4">
         <v>183</v>
       </c>
     </row>
     <row r="186" spans="2:2">
-      <c r="B186" s="7">
+      <c r="B186" s="4">
         <v>184</v>
       </c>
     </row>
     <row r="187" spans="2:2">
-      <c r="B187" s="7">
+      <c r="B187" s="4">
         <v>185</v>
       </c>
     </row>
     <row r="188" spans="2:2">
-      <c r="B188" s="7">
+      <c r="B188" s="4">
         <v>186</v>
       </c>
     </row>
     <row r="189" spans="2:2">
-      <c r="B189" s="7">
+      <c r="B189" s="4">
         <v>187</v>
       </c>
     </row>
     <row r="190" spans="2:2">
-      <c r="B190" s="7">
+      <c r="B190" s="4">
         <v>188</v>
       </c>
     </row>
     <row r="191" spans="2:2">
-      <c r="B191" s="7">
+      <c r="B191" s="4">
         <v>189</v>
       </c>
     </row>
     <row r="192" spans="2:2">
-      <c r="B192" s="7">
+      <c r="B192" s="4">
         <v>190</v>
       </c>
     </row>
     <row r="193" spans="2:2">
-      <c r="B193" s="7">
+      <c r="B193" s="4">
         <v>191</v>
       </c>
     </row>
     <row r="194" spans="2:2">
-      <c r="B194" s="7">
+      <c r="B194" s="4">
         <v>192</v>
       </c>
     </row>
     <row r="195" spans="2:2">
-      <c r="B195" s="7">
+      <c r="B195" s="4">
         <v>193</v>
       </c>
     </row>
     <row r="196" spans="2:2">
-      <c r="B196" s="7">
+      <c r="B196" s="4">
         <v>194</v>
       </c>
     </row>
     <row r="197" spans="2:2">
-      <c r="B197" s="7">
+      <c r="B197" s="4">
         <v>195</v>
       </c>
     </row>
     <row r="198" spans="2:2">
-      <c r="B198" s="7">
+      <c r="B198" s="4">
         <v>196</v>
       </c>
     </row>
     <row r="199" spans="2:2">
-      <c r="B199" s="7">
+      <c r="B199" s="4">
         <v>197</v>
       </c>
     </row>
     <row r="200" spans="2:2">
-      <c r="B200" s="7">
+      <c r="B200" s="4">
         <v>198</v>
       </c>
     </row>
     <row r="201" spans="2:2">
-      <c r="B201" s="7">
+      <c r="B201" s="4">
         <v>199</v>
       </c>
     </row>
     <row r="202" spans="2:2">
-      <c r="B202" s="7">
+      <c r="B202" s="4">
         <v>200</v>
       </c>
     </row>
     <row r="203" spans="2:2">
-      <c r="B203" s="7">
+      <c r="B203" s="4">
         <v>201</v>
       </c>
     </row>
     <row r="204" spans="2:2">
-      <c r="B204" s="7">
+      <c r="B204" s="4">
         <v>202</v>
       </c>
     </row>
     <row r="205" spans="2:2">
-      <c r="B205" s="7">
+      <c r="B205" s="4">
         <v>203</v>
       </c>
     </row>
     <row r="206" spans="2:2">
-      <c r="B206" s="7">
+      <c r="B206" s="4">
         <v>204</v>
       </c>
     </row>
     <row r="207" spans="2:2">
-      <c r="B207" s="7">
+      <c r="B207" s="4">
         <v>205</v>
       </c>
     </row>
     <row r="208" spans="2:2">
-      <c r="B208" s="7">
+      <c r="B208" s="4">
         <v>206</v>
       </c>
     </row>
     <row r="209" spans="2:2">
-      <c r="B209" s="7">
+      <c r="B209" s="4">
         <v>207</v>
       </c>
     </row>
     <row r="210" spans="2:2">
-      <c r="B210" s="7">
+      <c r="B210" s="4">
         <v>208</v>
       </c>
     </row>
     <row r="211" spans="2:2">
-      <c r="B211" s="7">
+      <c r="B211" s="4">
         <v>209</v>
       </c>
     </row>
     <row r="212" spans="2:2">
-      <c r="B212" s="7">
+      <c r="B212" s="4">
         <v>210</v>
       </c>
     </row>
     <row r="213" spans="2:2">
-      <c r="B213" s="7">
+      <c r="B213" s="4">
         <v>211</v>
       </c>
     </row>
     <row r="214" spans="2:2">
-      <c r="B214" s="7">
+      <c r="B214" s="4">
         <v>212</v>
       </c>
     </row>
     <row r="215" spans="2:2">
-      <c r="B215" s="7">
+      <c r="B215" s="4">
         <v>213</v>
       </c>
     </row>
     <row r="216" spans="2:2">
-      <c r="B216" s="7">
+      <c r="B216" s="4">
         <v>214</v>
       </c>
     </row>
     <row r="217" spans="2:2">
-      <c r="B217" s="7">
+      <c r="B217" s="4">
         <v>215</v>
       </c>
     </row>
     <row r="218" spans="2:2">
-      <c r="B218" s="7">
+      <c r="B218" s="4">
         <v>216</v>
       </c>
     </row>
     <row r="219" spans="2:2">
-      <c r="B219" s="7">
+      <c r="B219" s="4">
         <v>217</v>
       </c>
     </row>
     <row r="220" spans="2:2">
-      <c r="B220" s="7">
+      <c r="B220" s="4">
         <v>218</v>
       </c>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="7">
+      <c r="B221" s="4">
         <v>219</v>
       </c>
     </row>
     <row r="222" spans="2:2">
-      <c r="B222" s="7">
+      <c r="B222" s="4">
         <v>220</v>
       </c>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="7">
+      <c r="B223" s="4">
         <v>221</v>
       </c>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="7">
+      <c r="B224" s="4">
         <v>222</v>
       </c>
     </row>
     <row r="225" spans="2:5">
-      <c r="B225" s="7">
+      <c r="B225" s="4">
         <v>223</v>
       </c>
     </row>
     <row r="226" spans="2:5">
-      <c r="B226" s="7">
+      <c r="B226" s="4">
         <v>224</v>
       </c>
     </row>
     <row r="227" spans="2:5">
-      <c r="B227" s="7">
+      <c r="B227" s="4">
         <v>225</v>
       </c>
     </row>
     <row r="228" spans="2:5">
-      <c r="B228" s="7">
+      <c r="B228" s="4">
         <v>226</v>
       </c>
     </row>
     <row r="229" spans="2:5">
-      <c r="B229" s="7">
+      <c r="B229" s="4">
         <v>227</v>
       </c>
     </row>
     <row r="230" spans="2:5">
-      <c r="B230" s="7">
+      <c r="B230" s="4">
         <v>228</v>
       </c>
     </row>
     <row r="231" spans="2:5">
-      <c r="B231" s="7">
+      <c r="B231" s="4">
         <v>229</v>
       </c>
     </row>
     <row r="232" spans="2:5">
-      <c r="B232" s="7">
+      <c r="B232" s="4">
         <v>230</v>
       </c>
     </row>
     <row r="233" spans="2:5">
-      <c r="B233" s="7">
+      <c r="B233" s="4">
         <v>231</v>
       </c>
     </row>
     <row r="234" spans="2:5">
-      <c r="B234" s="7">
+      <c r="B234" s="4">
         <v>232</v>
       </c>
     </row>
     <row r="235" spans="2:5">
-      <c r="B235" s="7">
+      <c r="B235" s="4">
         <v>233</v>
       </c>
     </row>
     <row r="236" spans="2:5">
-      <c r="B236" s="7">
+      <c r="B236" s="4">
         <v>234</v>
       </c>
     </row>
     <row r="237" spans="2:5">
-      <c r="B237" s="7">
+      <c r="B237" s="4">
         <v>235</v>
       </c>
     </row>
     <row r="238" spans="2:5">
-      <c r="B238" s="7">
+      <c r="B238" s="4">
         <v>236</v>
       </c>
     </row>
     <row r="239" spans="2:5">
-      <c r="B239" s="7">
+      <c r="B239" s="4">
         <v>237</v>
       </c>
     </row>
     <row r="240" spans="2:5">
-      <c r="B240" s="8">
+      <c r="B240" s="5">
         <v>238</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D240" s="6">
+      <c r="D240" s="9">
         <v>41575</v>
       </c>
       <c r="E240" s="3" t="s">
@@ -2736,193 +2757,193 @@
       </c>
     </row>
     <row r="241" spans="2:2">
-      <c r="B241" s="7">
+      <c r="B241" s="4">
         <v>239</v>
       </c>
     </row>
     <row r="242" spans="2:2">
-      <c r="B242" s="7">
+      <c r="B242" s="4">
         <v>240</v>
       </c>
     </row>
     <row r="243" spans="2:2">
-      <c r="B243" s="7">
+      <c r="B243" s="4">
         <v>241</v>
       </c>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="7">
+      <c r="B244" s="4">
         <v>242</v>
       </c>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="7">
+      <c r="B245" s="4">
         <v>243</v>
       </c>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="7">
+      <c r="B246" s="4">
         <v>244</v>
       </c>
     </row>
     <row r="247" spans="2:2">
-      <c r="B247" s="7">
+      <c r="B247" s="4">
         <v>245</v>
       </c>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="7">
+      <c r="B248" s="4">
         <v>246</v>
       </c>
     </row>
     <row r="249" spans="2:2">
-      <c r="B249" s="7">
+      <c r="B249" s="4">
         <v>247</v>
       </c>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="7">
+      <c r="B250" s="4">
         <v>248</v>
       </c>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="7">
+      <c r="B251" s="4">
         <v>249</v>
       </c>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="7">
+      <c r="B252" s="4">
         <v>250</v>
       </c>
     </row>
     <row r="253" spans="2:2">
-      <c r="B253" s="7">
+      <c r="B253" s="4">
         <v>251</v>
       </c>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="7">
+      <c r="B254" s="4">
         <v>252</v>
       </c>
     </row>
     <row r="255" spans="2:2">
-      <c r="B255" s="7">
+      <c r="B255" s="4">
         <v>253</v>
       </c>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="7">
+      <c r="B256" s="4">
         <v>254</v>
       </c>
     </row>
     <row r="257" spans="2:2">
-      <c r="B257" s="7">
+      <c r="B257" s="4">
         <v>255</v>
       </c>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="7">
+      <c r="B258" s="4">
         <v>256</v>
       </c>
     </row>
     <row r="259" spans="2:2">
-      <c r="B259" s="7">
+      <c r="B259" s="4">
         <v>257</v>
       </c>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="7">
+      <c r="B260" s="4">
         <v>258</v>
       </c>
     </row>
     <row r="261" spans="2:2">
-      <c r="B261" s="7">
+      <c r="B261" s="4">
         <v>259</v>
       </c>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="7">
+      <c r="B262" s="4">
         <v>260</v>
       </c>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="7">
+      <c r="B263" s="4">
         <v>261</v>
       </c>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="7">
+      <c r="B264" s="4">
         <v>262</v>
       </c>
     </row>
     <row r="265" spans="2:2">
-      <c r="B265" s="7">
+      <c r="B265" s="4">
         <v>263</v>
       </c>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="7">
+      <c r="B266" s="4">
         <v>264</v>
       </c>
     </row>
     <row r="267" spans="2:2">
-      <c r="B267" s="7">
+      <c r="B267" s="4">
         <v>265</v>
       </c>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="7">
+      <c r="B268" s="4">
         <v>266</v>
       </c>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="7">
+      <c r="B269" s="4">
         <v>267</v>
       </c>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="7">
+      <c r="B270" s="4">
         <v>268</v>
       </c>
     </row>
     <row r="271" spans="2:2">
-      <c r="B271" s="7">
+      <c r="B271" s="4">
         <v>269</v>
       </c>
     </row>
     <row r="272" spans="2:2">
-      <c r="B272" s="7">
+      <c r="B272" s="4">
         <v>270</v>
       </c>
     </row>
     <row r="273" spans="2:5">
-      <c r="B273" s="7">
+      <c r="B273" s="4">
         <v>271</v>
       </c>
     </row>
     <row r="274" spans="2:5">
-      <c r="B274" s="7">
+      <c r="B274" s="4">
         <v>272</v>
       </c>
     </row>
     <row r="275" spans="2:5">
-      <c r="B275" s="7">
+      <c r="B275" s="4">
         <v>273</v>
       </c>
     </row>
     <row r="276" spans="2:5">
-      <c r="B276" s="7">
+      <c r="B276" s="4">
         <v>274</v>
       </c>
     </row>
     <row r="277" spans="2:5">
-      <c r="B277" s="8">
+      <c r="B277" s="5">
         <v>275</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D277" s="6">
+      <c r="D277" s="9">
         <v>41549</v>
       </c>
       <c r="E277" s="3" t="s">
@@ -2930,233 +2951,233 @@
       </c>
     </row>
     <row r="278" spans="2:5">
-      <c r="B278" s="7">
+      <c r="B278" s="4">
         <v>276</v>
       </c>
     </row>
     <row r="279" spans="2:5">
-      <c r="B279" s="7">
+      <c r="B279" s="4">
         <v>277</v>
       </c>
     </row>
     <row r="280" spans="2:5">
-      <c r="B280" s="7">
+      <c r="B280" s="4">
         <v>278</v>
       </c>
     </row>
     <row r="281" spans="2:5">
-      <c r="B281" s="7">
+      <c r="B281" s="4">
         <v>279</v>
       </c>
     </row>
     <row r="282" spans="2:5">
-      <c r="B282" s="7">
+      <c r="B282" s="4">
         <v>280</v>
       </c>
     </row>
     <row r="283" spans="2:5">
-      <c r="B283" s="7">
+      <c r="B283" s="4">
         <v>281</v>
       </c>
     </row>
     <row r="284" spans="2:5">
-      <c r="B284" s="7">
+      <c r="B284" s="4">
         <v>282</v>
       </c>
     </row>
     <row r="285" spans="2:5">
-      <c r="B285" s="7">
+      <c r="B285" s="4">
         <v>283</v>
       </c>
     </row>
     <row r="286" spans="2:5">
-      <c r="B286" s="7">
+      <c r="B286" s="4">
         <v>284</v>
       </c>
     </row>
     <row r="287" spans="2:5">
-      <c r="B287" s="7">
+      <c r="B287" s="4">
         <v>285</v>
       </c>
     </row>
     <row r="288" spans="2:5">
-      <c r="B288" s="7">
+      <c r="B288" s="4">
         <v>286</v>
       </c>
     </row>
     <row r="289" spans="2:2">
-      <c r="B289" s="7">
+      <c r="B289" s="4">
         <v>287</v>
       </c>
     </row>
     <row r="290" spans="2:2">
-      <c r="B290" s="7">
+      <c r="B290" s="4">
         <v>288</v>
       </c>
     </row>
     <row r="291" spans="2:2">
-      <c r="B291" s="7">
+      <c r="B291" s="4">
         <v>289</v>
       </c>
     </row>
     <row r="292" spans="2:2">
-      <c r="B292" s="7">
+      <c r="B292" s="4">
         <v>290</v>
       </c>
     </row>
     <row r="293" spans="2:2">
-      <c r="B293" s="7">
+      <c r="B293" s="4">
         <v>291</v>
       </c>
     </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="7">
+      <c r="B294" s="4">
         <v>292</v>
       </c>
     </row>
     <row r="295" spans="2:2">
-      <c r="B295" s="7">
+      <c r="B295" s="4">
         <v>293</v>
       </c>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="7">
+      <c r="B296" s="4">
         <v>294</v>
       </c>
     </row>
     <row r="297" spans="2:2">
-      <c r="B297" s="7">
+      <c r="B297" s="4">
         <v>295</v>
       </c>
     </row>
     <row r="298" spans="2:2">
-      <c r="B298" s="7">
+      <c r="B298" s="4">
         <v>296</v>
       </c>
     </row>
     <row r="299" spans="2:2">
-      <c r="B299" s="7">
+      <c r="B299" s="4">
         <v>297</v>
       </c>
     </row>
     <row r="300" spans="2:2">
-      <c r="B300" s="7">
+      <c r="B300" s="4">
         <v>298</v>
       </c>
     </row>
     <row r="301" spans="2:2">
-      <c r="B301" s="7">
+      <c r="B301" s="4">
         <v>299</v>
       </c>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="7">
+      <c r="B302" s="4">
         <v>300</v>
       </c>
     </row>
     <row r="303" spans="2:2">
-      <c r="B303" s="7">
+      <c r="B303" s="4">
         <v>301</v>
       </c>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="7">
+      <c r="B304" s="4">
         <v>302</v>
       </c>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="7">
+      <c r="B305" s="4">
         <v>303</v>
       </c>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="7">
+      <c r="B306" s="4">
         <v>304</v>
       </c>
     </row>
     <row r="307" spans="2:2">
-      <c r="B307" s="7">
+      <c r="B307" s="4">
         <v>305</v>
       </c>
     </row>
     <row r="308" spans="2:2">
-      <c r="B308" s="7">
+      <c r="B308" s="4">
         <v>306</v>
       </c>
     </row>
     <row r="309" spans="2:2">
-      <c r="B309" s="7">
+      <c r="B309" s="4">
         <v>307</v>
       </c>
     </row>
     <row r="310" spans="2:2">
-      <c r="B310" s="7">
+      <c r="B310" s="4">
         <v>308</v>
       </c>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="7">
+      <c r="B311" s="4">
         <v>309</v>
       </c>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="7">
+      <c r="B312" s="4">
         <v>310</v>
       </c>
     </row>
     <row r="313" spans="2:2">
-      <c r="B313" s="7">
+      <c r="B313" s="4">
         <v>311</v>
       </c>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="7">
+      <c r="B314" s="4">
         <v>312</v>
       </c>
     </row>
     <row r="315" spans="2:2">
-      <c r="B315" s="7">
+      <c r="B315" s="4">
         <v>313</v>
       </c>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="7">
+      <c r="B316" s="4">
         <v>314</v>
       </c>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="7">
+      <c r="B317" s="4">
         <v>315</v>
       </c>
     </row>
     <row r="318" spans="2:2">
-      <c r="B318" s="7">
+      <c r="B318" s="4">
         <v>316</v>
       </c>
     </row>
     <row r="319" spans="2:2">
-      <c r="B319" s="7">
+      <c r="B319" s="4">
         <v>317</v>
       </c>
     </row>
     <row r="320" spans="2:2">
-      <c r="B320" s="7">
+      <c r="B320" s="4">
         <v>318</v>
       </c>
     </row>
     <row r="321" spans="2:5">
-      <c r="B321" s="7">
+      <c r="B321" s="4">
         <v>319</v>
       </c>
     </row>
     <row r="322" spans="2:5">
-      <c r="B322" s="8">
+      <c r="B322" s="5">
         <v>320</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D322" s="6">
+      <c r="D322" s="9">
         <v>41548</v>
       </c>
       <c r="E322" s="3" t="s">
@@ -3164,487 +3185,487 @@
       </c>
     </row>
     <row r="323" spans="2:5">
-      <c r="B323" s="7">
+      <c r="B323" s="4">
         <v>321</v>
       </c>
     </row>
     <row r="324" spans="2:5">
-      <c r="B324" s="7">
+      <c r="B324" s="4">
         <v>322</v>
       </c>
     </row>
     <row r="325" spans="2:5">
-      <c r="B325" s="7">
+      <c r="B325" s="4">
         <v>323</v>
       </c>
     </row>
     <row r="326" spans="2:5">
-      <c r="B326" s="7">
+      <c r="B326" s="4">
         <v>324</v>
       </c>
     </row>
     <row r="327" spans="2:5">
-      <c r="B327" s="7">
+      <c r="B327" s="4">
         <v>325</v>
       </c>
     </row>
     <row r="328" spans="2:5">
-      <c r="B328" s="7">
+      <c r="B328" s="4">
         <v>326</v>
       </c>
     </row>
     <row r="329" spans="2:5">
-      <c r="B329" s="7">
+      <c r="B329" s="4">
         <v>327</v>
       </c>
     </row>
     <row r="330" spans="2:5">
-      <c r="B330" s="7">
+      <c r="B330" s="4">
         <v>328</v>
       </c>
     </row>
     <row r="331" spans="2:5">
-      <c r="B331" s="7">
+      <c r="B331" s="4">
         <v>329</v>
       </c>
     </row>
     <row r="332" spans="2:5">
-      <c r="B332" s="7">
+      <c r="B332" s="4">
         <v>330</v>
       </c>
     </row>
     <row r="333" spans="2:5">
-      <c r="B333" s="7">
+      <c r="B333" s="4">
         <v>331</v>
       </c>
     </row>
     <row r="334" spans="2:5">
-      <c r="B334" s="7">
+      <c r="B334" s="4">
         <v>332</v>
       </c>
     </row>
     <row r="335" spans="2:5">
-      <c r="B335" s="7">
+      <c r="B335" s="4">
         <v>333</v>
       </c>
     </row>
     <row r="336" spans="2:5">
-      <c r="B336" s="7">
+      <c r="B336" s="4">
         <v>334</v>
       </c>
     </row>
     <row r="337" spans="2:2">
-      <c r="B337" s="7">
+      <c r="B337" s="4">
         <v>335</v>
       </c>
     </row>
     <row r="338" spans="2:2">
-      <c r="B338" s="7">
+      <c r="B338" s="4">
         <v>336</v>
       </c>
     </row>
     <row r="339" spans="2:2">
-      <c r="B339" s="7">
+      <c r="B339" s="4">
         <v>337</v>
       </c>
     </row>
     <row r="340" spans="2:2">
-      <c r="B340" s="7">
+      <c r="B340" s="4">
         <v>338</v>
       </c>
     </row>
     <row r="341" spans="2:2">
-      <c r="B341" s="7">
+      <c r="B341" s="4">
         <v>339</v>
       </c>
     </row>
     <row r="342" spans="2:2">
-      <c r="B342" s="7">
+      <c r="B342" s="4">
         <v>340</v>
       </c>
     </row>
     <row r="343" spans="2:2">
-      <c r="B343" s="7">
+      <c r="B343" s="4">
         <v>341</v>
       </c>
     </row>
     <row r="344" spans="2:2">
-      <c r="B344" s="7">
+      <c r="B344" s="4">
         <v>342</v>
       </c>
     </row>
     <row r="345" spans="2:2">
-      <c r="B345" s="7">
+      <c r="B345" s="4">
         <v>343</v>
       </c>
     </row>
     <row r="346" spans="2:2">
-      <c r="B346" s="7">
+      <c r="B346" s="4">
         <v>344</v>
       </c>
     </row>
     <row r="347" spans="2:2">
-      <c r="B347" s="7">
+      <c r="B347" s="4">
         <v>345</v>
       </c>
     </row>
     <row r="348" spans="2:2">
-      <c r="B348" s="7">
+      <c r="B348" s="4">
         <v>346</v>
       </c>
     </row>
     <row r="349" spans="2:2">
-      <c r="B349" s="7">
+      <c r="B349" s="4">
         <v>347</v>
       </c>
     </row>
     <row r="350" spans="2:2">
-      <c r="B350" s="7">
+      <c r="B350" s="4">
         <v>348</v>
       </c>
     </row>
     <row r="351" spans="2:2">
-      <c r="B351" s="7">
+      <c r="B351" s="4">
         <v>349</v>
       </c>
     </row>
     <row r="352" spans="2:2">
-      <c r="B352" s="7">
+      <c r="B352" s="4">
         <v>350</v>
       </c>
     </row>
     <row r="353" spans="2:2">
-      <c r="B353" s="7">
+      <c r="B353" s="4">
         <v>351</v>
       </c>
     </row>
     <row r="354" spans="2:2">
-      <c r="B354" s="7">
+      <c r="B354" s="4">
         <v>352</v>
       </c>
     </row>
     <row r="355" spans="2:2">
-      <c r="B355" s="7">
+      <c r="B355" s="4">
         <v>353</v>
       </c>
     </row>
     <row r="356" spans="2:2">
-      <c r="B356" s="7">
+      <c r="B356" s="4">
         <v>354</v>
       </c>
     </row>
     <row r="357" spans="2:2">
-      <c r="B357" s="7">
+      <c r="B357" s="4">
         <v>355</v>
       </c>
     </row>
     <row r="358" spans="2:2">
-      <c r="B358" s="7">
+      <c r="B358" s="4">
         <v>356</v>
       </c>
     </row>
     <row r="359" spans="2:2">
-      <c r="B359" s="7">
+      <c r="B359" s="4">
         <v>357</v>
       </c>
     </row>
     <row r="360" spans="2:2">
-      <c r="B360" s="7">
+      <c r="B360" s="4">
         <v>358</v>
       </c>
     </row>
     <row r="361" spans="2:2">
-      <c r="B361" s="7">
+      <c r="B361" s="4">
         <v>359</v>
       </c>
     </row>
     <row r="362" spans="2:2">
-      <c r="B362" s="7">
+      <c r="B362" s="4">
         <v>360</v>
       </c>
     </row>
     <row r="363" spans="2:2">
-      <c r="B363" s="7">
+      <c r="B363" s="4">
         <v>361</v>
       </c>
     </row>
     <row r="364" spans="2:2">
-      <c r="B364" s="7">
+      <c r="B364" s="4">
         <v>362</v>
       </c>
     </row>
     <row r="365" spans="2:2">
-      <c r="B365" s="7">
+      <c r="B365" s="4">
         <v>363</v>
       </c>
     </row>
     <row r="366" spans="2:2">
-      <c r="B366" s="7">
+      <c r="B366" s="4">
         <v>364</v>
       </c>
     </row>
     <row r="367" spans="2:2">
-      <c r="B367" s="7">
+      <c r="B367" s="4">
         <v>365</v>
       </c>
     </row>
     <row r="368" spans="2:2">
-      <c r="B368" s="7">
+      <c r="B368" s="4">
         <v>366</v>
       </c>
     </row>
     <row r="369" spans="2:2">
-      <c r="B369" s="7">
+      <c r="B369" s="4">
         <v>367</v>
       </c>
     </row>
     <row r="370" spans="2:2">
-      <c r="B370" s="7">
+      <c r="B370" s="4">
         <v>368</v>
       </c>
     </row>
     <row r="371" spans="2:2">
-      <c r="B371" s="7">
+      <c r="B371" s="4">
         <v>369</v>
       </c>
     </row>
     <row r="372" spans="2:2">
-      <c r="B372" s="7">
+      <c r="B372" s="4">
         <v>370</v>
       </c>
     </row>
     <row r="373" spans="2:2">
-      <c r="B373" s="7">
+      <c r="B373" s="4">
         <v>371</v>
       </c>
     </row>
     <row r="374" spans="2:2">
-      <c r="B374" s="7">
+      <c r="B374" s="4">
         <v>372</v>
       </c>
     </row>
     <row r="375" spans="2:2">
-      <c r="B375" s="7">
+      <c r="B375" s="4">
         <v>373</v>
       </c>
     </row>
     <row r="376" spans="2:2">
-      <c r="B376" s="7">
+      <c r="B376" s="4">
         <v>374</v>
       </c>
     </row>
     <row r="377" spans="2:2">
-      <c r="B377" s="7">
+      <c r="B377" s="4">
         <v>375</v>
       </c>
     </row>
     <row r="378" spans="2:2">
-      <c r="B378" s="7">
+      <c r="B378" s="4">
         <v>376</v>
       </c>
     </row>
     <row r="379" spans="2:2">
-      <c r="B379" s="7">
+      <c r="B379" s="4">
         <v>377</v>
       </c>
     </row>
     <row r="380" spans="2:2">
-      <c r="B380" s="7">
+      <c r="B380" s="4">
         <v>378</v>
       </c>
     </row>
     <row r="381" spans="2:2">
-      <c r="B381" s="7">
+      <c r="B381" s="4">
         <v>379</v>
       </c>
     </row>
     <row r="382" spans="2:2">
-      <c r="B382" s="7">
+      <c r="B382" s="4">
         <v>380</v>
       </c>
     </row>
     <row r="383" spans="2:2">
-      <c r="B383" s="7">
+      <c r="B383" s="4">
         <v>381</v>
       </c>
     </row>
     <row r="384" spans="2:2">
-      <c r="B384" s="7">
+      <c r="B384" s="4">
         <v>382</v>
       </c>
     </row>
     <row r="385" spans="2:2">
-      <c r="B385" s="7">
+      <c r="B385" s="4">
         <v>383</v>
       </c>
     </row>
     <row r="386" spans="2:2">
-      <c r="B386" s="7">
+      <c r="B386" s="4">
         <v>384</v>
       </c>
     </row>
     <row r="387" spans="2:2">
-      <c r="B387" s="7">
+      <c r="B387" s="4">
         <v>385</v>
       </c>
     </row>
     <row r="388" spans="2:2">
-      <c r="B388" s="7">
+      <c r="B388" s="4">
         <v>386</v>
       </c>
     </row>
     <row r="389" spans="2:2">
-      <c r="B389" s="7">
+      <c r="B389" s="4">
         <v>387</v>
       </c>
     </row>
     <row r="390" spans="2:2">
-      <c r="B390" s="7">
+      <c r="B390" s="4">
         <v>388</v>
       </c>
     </row>
     <row r="391" spans="2:2">
-      <c r="B391" s="7">
+      <c r="B391" s="4">
         <v>389</v>
       </c>
     </row>
     <row r="392" spans="2:2">
-      <c r="B392" s="7">
+      <c r="B392" s="4">
         <v>390</v>
       </c>
     </row>
     <row r="393" spans="2:2">
-      <c r="B393" s="7">
+      <c r="B393" s="4">
         <v>391</v>
       </c>
     </row>
     <row r="394" spans="2:2">
-      <c r="B394" s="7">
+      <c r="B394" s="4">
         <v>392</v>
       </c>
     </row>
     <row r="395" spans="2:2">
-      <c r="B395" s="7">
+      <c r="B395" s="4">
         <v>393</v>
       </c>
     </row>
     <row r="396" spans="2:2">
-      <c r="B396" s="7">
+      <c r="B396" s="4">
         <v>394</v>
       </c>
     </row>
     <row r="397" spans="2:2">
-      <c r="B397" s="7">
+      <c r="B397" s="4">
         <v>395</v>
       </c>
     </row>
     <row r="398" spans="2:2">
-      <c r="B398" s="7">
+      <c r="B398" s="4">
         <v>396</v>
       </c>
     </row>
     <row r="399" spans="2:2">
-      <c r="B399" s="7">
+      <c r="B399" s="4">
         <v>397</v>
       </c>
     </row>
     <row r="400" spans="2:2">
-      <c r="B400" s="7">
+      <c r="B400" s="4">
         <v>398</v>
       </c>
     </row>
     <row r="401" spans="2:2">
-      <c r="B401" s="7">
+      <c r="B401" s="4">
         <v>399</v>
       </c>
     </row>
     <row r="402" spans="2:2">
-      <c r="B402" s="7">
+      <c r="B402" s="4">
         <v>400</v>
       </c>
     </row>
     <row r="403" spans="2:2">
-      <c r="B403" s="7">
+      <c r="B403" s="4">
         <v>401</v>
       </c>
     </row>
     <row r="404" spans="2:2">
-      <c r="B404" s="7">
+      <c r="B404" s="4">
         <v>402</v>
       </c>
     </row>
     <row r="405" spans="2:2">
-      <c r="B405" s="7">
+      <c r="B405" s="4">
         <v>403</v>
       </c>
     </row>
     <row r="406" spans="2:2">
-      <c r="B406" s="7">
+      <c r="B406" s="4">
         <v>404</v>
       </c>
     </row>
     <row r="407" spans="2:2">
-      <c r="B407" s="7">
+      <c r="B407" s="4">
         <v>405</v>
       </c>
     </row>
     <row r="408" spans="2:2">
-      <c r="B408" s="7">
+      <c r="B408" s="4">
         <v>406</v>
       </c>
     </row>
     <row r="409" spans="2:2">
-      <c r="B409" s="7">
+      <c r="B409" s="4">
         <v>407</v>
       </c>
     </row>
     <row r="410" spans="2:2">
-      <c r="B410" s="7">
+      <c r="B410" s="4">
         <v>408</v>
       </c>
     </row>
     <row r="411" spans="2:2">
-      <c r="B411" s="7">
+      <c r="B411" s="4">
         <v>409</v>
       </c>
     </row>
     <row r="412" spans="2:2">
-      <c r="B412" s="7">
+      <c r="B412" s="4">
         <v>410</v>
       </c>
     </row>
     <row r="413" spans="2:2">
-      <c r="B413" s="7">
+      <c r="B413" s="4">
         <v>411</v>
       </c>
     </row>
     <row r="414" spans="2:2">
-      <c r="B414" s="7">
+      <c r="B414" s="4">
         <v>412</v>
       </c>
     </row>
     <row r="415" spans="2:2">
-      <c r="B415" s="7">
+      <c r="B415" s="4">
         <v>413</v>
       </c>
     </row>
     <row r="416" spans="2:2">
-      <c r="B416" s="7">
+      <c r="B416" s="4">
         <v>414</v>
       </c>
     </row>
     <row r="417" spans="2:2">
-      <c r="B417" s="7">
+      <c r="B417" s="4">
         <v>415</v>
       </c>
     </row>
     <row r="418" spans="2:2">
-      <c r="B418" s="7">
+      <c r="B418" s="4">
         <v>416</v>
       </c>
     </row>
     <row r="419" spans="2:2">
-      <c r="B419" s="7">
+      <c r="B419" s="4">
         <v>417</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 026.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="271">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -830,6 +830,12 @@
   </si>
   <si>
     <t>Use ? to prevent SQL Injection - e.g. Model.where(["name LIKE ?", "%#{params[:query]}%"])</t>
+  </si>
+  <si>
+    <t>Hackers Love Mass Assignment</t>
+  </si>
+  <si>
+    <t>For Rails &lt;= 3.X, use attr_accessible to whitelist attributes for mass assignment.</t>
   </si>
 </sst>
 </file>
@@ -837,7 +843,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -893,8 +899,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -935,20 +943,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -959,6 +967,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -969,6 +978,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1304,7 +1314,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1683,8 +1693,17 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="4">
+      <c r="B28" s="5">
         <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="6">
+        <v>42007</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 027, 028, 029, 030.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -899,8 +899,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -956,7 +960,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -968,6 +972,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -979,6 +985,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1314,7 +1322,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1707,23 +1715,35 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="4">
+      <c r="B29" s="5">
         <v>27</v>
       </c>
+      <c r="D29" s="6">
+        <v>42009</v>
+      </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="4">
+      <c r="B30" s="5">
         <v>28</v>
       </c>
+      <c r="D30" s="6">
+        <v>42009</v>
+      </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="4">
+      <c r="B31" s="5">
         <v>29</v>
       </c>
+      <c r="D31" s="6">
+        <v>42009</v>
+      </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="4">
+      <c r="B32" s="5">
         <v>30</v>
+      </c>
+      <c r="D32" s="6">
+        <v>42009</v>
       </c>
     </row>
     <row r="33" spans="2:2">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 031, 032.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="283">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -836,6 +836,42 @@
   </si>
   <si>
     <t>For Rails &lt;= 3.X, use attr_accessible to whitelist attributes for mass assignment.</t>
+  </si>
+  <si>
+    <t>Use h method in views and CGI::escape method in controllers to prevent CSS from happening.</t>
+  </si>
+  <si>
+    <t>Use in_group_of to split array into subarrays: &lt;% @tasks.in_groups_of(4, false) do |row_tasks| %&gt;</t>
+  </si>
+  <si>
+    <t>group_by</t>
+  </si>
+  <si>
+    <t>Use group_by { |e| e.send(:method) } to group elements by criteria into key-value pairs.</t>
+  </si>
+  <si>
+    <t>Pretty Page Title</t>
+  </si>
+  <si>
+    <t>Create a title method in ApplicationHelper to assist in page titles: content_for(:title) { page_title }</t>
+  </si>
+  <si>
+    <t>Cross Site Scripting</t>
+  </si>
+  <si>
+    <t>in_groups_of</t>
+  </si>
+  <si>
+    <t>Formatting Time</t>
+  </si>
+  <si>
+    <t>In environment.rb =&gt; Time::DATE_FORMATS[:due_time] = "due on %B %d at %I:%M %p"</t>
+  </si>
+  <si>
+    <t>Time in Text Field</t>
+  </si>
+  <si>
+    <t>Use virtual attributes (getter/setter) &amp; custom validations to properly parse and display time in text.</t>
   </si>
 </sst>
 </file>
@@ -899,8 +935,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -960,7 +1000,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -974,6 +1014,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -987,6 +1029,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1322,7 +1366,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1718,110 +1762,152 @@
       <c r="B29" s="5">
         <v>27</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="D29" s="6">
         <v>42009</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5">
         <v>28</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="D30" s="6">
         <v>42009</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5">
         <v>29</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D31" s="6">
         <v>42009</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="5">
         <v>30</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="D32" s="6">
         <v>42009</v>
       </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="4">
+      <c r="E32" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="5">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="4">
+      <c r="C33" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D33" s="6">
+        <v>42012</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="C34" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D34" s="6">
+        <v>42013</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:5">
       <c r="B36" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:5">
       <c r="B37" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:5">
       <c r="B38" s="4">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:5">
       <c r="B39" s="4">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:5">
       <c r="B40" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:5">
       <c r="B41" s="4">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:5">
       <c r="B42" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:5">
       <c r="B43" s="4">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:5">
       <c r="B44" s="4">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:5">
       <c r="B45" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:5">
       <c r="B46" s="4">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:5">
       <c r="B47" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:5">
       <c r="B48" s="4">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 033.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="285">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -872,6 +872,12 @@
   </si>
   <si>
     <t>Use virtual attributes (getter/setter) &amp; custom validations to properly parse and display time in text.</t>
+  </si>
+  <si>
+    <t>Making a Plugin</t>
+  </si>
+  <si>
+    <t>Plugins can be made to provide functionality to models (encapsulate code) [e.g. ActiveRecord].</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1369,7 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
@@ -1843,8 +1849,17 @@
       </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="4">
+      <c r="B35" s="5">
         <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D35" s="6">
+        <v>42016</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 034.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="287">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -878,6 +878,12 @@
   </si>
   <si>
     <t>Plugins can be made to provide functionality to models (encapsulate code) [e.g. ActiveRecord].</t>
+  </si>
+  <si>
+    <t>Named Routes</t>
+  </si>
+  <si>
+    <t>[OBE] map.named_route can be used in &lt;= Rails 2 to define a name route (*_path &amp; *_url).</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1378,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1863,8 +1869,17 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="4">
+      <c r="B36" s="5">
         <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D36" s="6">
+        <v>42017</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 035, 036, 037.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="293">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -884,6 +884,24 @@
   </si>
   <si>
     <t>[OBE] map.named_route can be used in &lt;= Rails 2 to define a name route (*_path &amp; *_url).</t>
+  </si>
+  <si>
+    <t>Custom REST Actions</t>
+  </si>
+  <si>
+    <t>Create :member / :collection routes in routes.rb for custom controller actions =&gt; "REST is best!"</t>
+  </si>
+  <si>
+    <t>Subversion on Rails</t>
+  </si>
+  <si>
+    <t>[OBE] Instructions on how to setup Subversion in Rails =&gt; Git is now the 'global' preference.</t>
+  </si>
+  <si>
+    <t>Simple Search Form</t>
+  </si>
+  <si>
+    <t>Use form_tag // GET to request info from #index, create Model.search to encapsulate logic.</t>
   </si>
 </sst>
 </file>
@@ -947,8 +965,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1012,7 +1034,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1028,6 +1050,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1043,6 +1067,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1378,7 +1404,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1883,18 +1909,45 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="4">
+      <c r="B37" s="5">
         <v>35</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37" s="6">
+        <v>42022</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="4">
+      <c r="B38" s="5">
         <v>36</v>
       </c>
+      <c r="C38" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D38" s="6">
+        <v>42022</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="4">
+      <c r="B39" s="5">
         <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D39" s="6">
+        <v>42022</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 038, 039.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="297">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -902,6 +902,18 @@
   </si>
   <si>
     <t>Use form_tag // GET to request info from #index, create Model.search to encapsulate logic.</t>
+  </si>
+  <si>
+    <t>Multibutton Form</t>
+  </si>
+  <si>
+    <t>Name the new button and check for it in controller (e.g. params[:preview_button] || !@project.save).</t>
+  </si>
+  <si>
+    <t>Customize Field Error</t>
+  </si>
+  <si>
+    <t>[OBE] ActionView::Base.field_error_proc = Proc.new do |html_tag, instance_tag| in environment.rb</t>
   </si>
 </sst>
 </file>
@@ -965,8 +977,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1034,7 +1048,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1052,6 +1066,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1069,6 +1084,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1404,7 +1420,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1951,13 +1967,31 @@
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="4">
+      <c r="B40" s="5">
         <v>38</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D40" s="6">
+        <v>42023</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="4">
+      <c r="B41" s="5">
         <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D41" s="6">
+        <v>42023</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 040.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="299">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -914,6 +914,12 @@
   </si>
   <si>
     <t>[OBE] ActionView::Base.field_error_proc = Proc.new do |html_tag, instance_tag| in environment.rb</t>
+  </si>
+  <si>
+    <t>Blocks in View</t>
+  </si>
+  <si>
+    <t>[OBE] concat content_tag(:div, capture(&amp;block), :class =&gt; 'admin'), block.binding if admin?</t>
   </si>
 </sst>
 </file>
@@ -977,8 +983,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1048,7 +1056,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1067,6 +1075,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1085,6 +1094,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1420,7 +1430,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1995,8 +2005,17 @@
       </c>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="4">
+      <c r="B42" s="5">
         <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D42" s="6">
+        <v>42023</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 041, 042.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="303">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -920,6 +920,18 @@
   </si>
   <si>
     <t>[OBE] concat content_tag(:div, capture(&amp;block), :class =&gt; 'admin'), block.binding if admin?</t>
+  </si>
+  <si>
+    <t>Conditional Validations</t>
+  </si>
+  <si>
+    <t>Define methods on validations (:if =&gt; :should_validate_password?) &amp; attr_accessor in controllers.</t>
+  </si>
+  <si>
+    <t>Use with_options (with_options :if =&gt; :should_validate_password? do |user|) to remove duplication.</t>
+  </si>
+  <si>
+    <t>with_options</t>
   </si>
 </sst>
 </file>
@@ -983,8 +995,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1056,7 +1070,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1076,6 +1090,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1095,6 +1110,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,10 +1443,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2019,13 +2035,31 @@
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="4">
+      <c r="B43" s="5">
         <v>41</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D43" s="6">
+        <v>42024</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="4">
+      <c r="B44" s="5">
         <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D44" s="6">
+        <v>42024</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 043.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="305">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -932,6 +932,12 @@
   </si>
   <si>
     <t>with_options</t>
+  </si>
+  <si>
+    <t>AJAX with RJS</t>
+  </si>
+  <si>
+    <t>RJS (now UJS) can be used to return JS to the client from controller which will be executed inline.</t>
   </si>
 </sst>
 </file>
@@ -1443,10 +1449,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2063,8 +2069,17 @@
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="4">
+      <c r="B45" s="5">
         <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D45" s="6">
+        <v>42037</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 044, 045.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="309">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -938,6 +938,18 @@
   </si>
   <si>
     <t>RJS (now UJS) can be used to return JS to the client from controller which will be executed inline.</t>
+  </si>
+  <si>
+    <t>Debugging RJS</t>
+  </si>
+  <si>
+    <t>RJS (UJS) should be debugged by looking at development log for immediate issues, then in JS.</t>
+  </si>
+  <si>
+    <t>RJS Tips</t>
+  </si>
+  <si>
+    <t>[OBE] RJS (UJS) templating tips are show in this RailsCasts but are no longer the default.</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1013,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1076,7 +1094,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1097,6 +1115,9 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1117,6 +1138,9 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1452,7 +1476,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2083,13 +2107,31 @@
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="4">
+      <c r="B46" s="5">
         <v>44</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="6">
+        <v>42038</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="4">
+      <c r="B47" s="5">
         <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D47" s="6">
+        <v>42038</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 046, 047.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="313">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -950,6 +950,18 @@
   </si>
   <si>
     <t>[OBE] RJS (UJS) templating tips are show in this RailsCasts but are no longer the default.</t>
+  </si>
+  <si>
+    <t>Catch-all Route</t>
+  </si>
+  <si>
+    <t>Add in a 'match *' route in routes.rb to deal with things like redirects or unintended routes.</t>
+  </si>
+  <si>
+    <t>Two Many-to-Many</t>
+  </si>
+  <si>
+    <t>Use HABTM when only foreign keys are needed in join table and has_many :through otherwise.</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1025,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1094,7 +1108,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1118,6 +1132,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1141,6 +1156,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1476,7 +1492,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2135,86 +2151,104 @@
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="4">
+      <c r="B48" s="5">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="4">
+      <c r="C48" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D48" s="6">
+        <v>42039</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="5">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="2:2">
+      <c r="C49" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D49" s="6">
+        <v>42039</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="4">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:5">
       <c r="B51" s="4">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:5">
       <c r="B52" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:5">
       <c r="B53" s="4">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="2:5">
       <c r="B54" s="4">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:5">
       <c r="B55" s="4">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="2:5">
       <c r="B56" s="4">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:5">
       <c r="B57" s="4">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="2:5">
       <c r="B58" s="4">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="2:5">
       <c r="B59" s="4">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:2">
+    <row r="60" spans="2:5">
       <c r="B60" s="4">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="2:5">
       <c r="B61" s="4">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="2:5">
       <c r="B62" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
+    <row r="63" spans="2:5">
       <c r="B63" s="4">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="2:5">
       <c r="B64" s="4">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 048.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="315">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -962,6 +962,12 @@
   </si>
   <si>
     <t>Use HABTM when only foreign keys are needed in join table and has_many :through otherwise.</t>
+  </si>
+  <si>
+    <t>Console Tricks</t>
+  </si>
+  <si>
+    <t>Use a bunch of useful tricks (e.g. rails c --sandbox // app.user_path) when in Rails console.</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1495,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2179,8 +2185,17 @@
       </c>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="4">
+      <c r="B50" s="5">
         <v>48</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D50" s="6">
+        <v>42045</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 417.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="317">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>Use a bunch of useful tricks (e.g. rails c --sandbox // app.user_path) when in Rails console.</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Foundation is a mobile-first,responsive, FED-library based on SCSS - easily integrates with Rails.</t>
   </si>
 </sst>
 </file>
@@ -1495,10 +1501,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B412" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="E419" sqref="E419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4055,19 +4061,28 @@
         <v>414</v>
       </c>
     </row>
-    <row r="417" spans="2:2">
+    <row r="417" spans="2:5">
       <c r="B417" s="4">
         <v>415</v>
       </c>
     </row>
-    <row r="418" spans="2:2">
+    <row r="418" spans="2:5">
       <c r="B418" s="4">
         <v>416</v>
       </c>
     </row>
-    <row r="419" spans="2:2">
-      <c r="B419" s="4">
+    <row r="419" spans="2:5">
+      <c r="B419" s="5">
         <v>417</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D419" s="6">
+        <v>42049</v>
+      </c>
+      <c r="E419" s="3" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 049.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="319">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -974,6 +974,12 @@
   </si>
   <si>
     <t>Foundation is a mobile-first,responsive, FED-library based on SCSS - easily integrates with Rails.</t>
+  </si>
+  <si>
+    <t>Reading the API</t>
+  </si>
+  <si>
+    <t>Head to http://api.rubyonrails.org/ for additional info on Rails declarations (other options as well).</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1043,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1120,7 +1128,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1145,6 +1153,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1169,6 +1178,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1501,10 +1511,10 @@
   <dimension ref="B1:E419"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B412" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E419" sqref="E419"/>
+      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2205,8 +2215,17 @@
       </c>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="4">
+      <c r="B51" s="5">
         <v>49</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D51" s="6">
+        <v>42051</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 048, 049, 050.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="-2000" yWindow="-21440" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="325">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -980,6 +980,24 @@
   </si>
   <si>
     <t>Head to http://api.rubyonrails.org/ for additional info on Rails declarations (other options as well).</t>
+  </si>
+  <si>
+    <t>Contributing to Rails</t>
+  </si>
+  <si>
+    <t>[OBE] Tips on how to submit patches to legacy Rails code base.</t>
+  </si>
+  <si>
+    <t>will_paginate</t>
+  </si>
+  <si>
+    <t>Use the will_paginate gem to provide custom pagination cross different Rails pages.</t>
+  </si>
+  <si>
+    <t>Update through Checkboxes</t>
+  </si>
+  <si>
+    <t>Create form_tags to post multiple checkbox IDs to controllers where update actions are exectued.</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1061,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1128,7 +1150,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1154,6 +1176,8 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1179,6 +1203,8 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1514,7 +1540,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2229,18 +2255,45 @@
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="4">
+      <c r="B52" s="5">
         <v>50</v>
       </c>
+      <c r="C52" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D52" s="6">
+        <v>42073</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="4">
+      <c r="B53" s="5">
         <v>51</v>
       </c>
+      <c r="C53" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D53" s="6">
+        <v>42073</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="4">
+      <c r="B54" s="5">
         <v>52</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D54" s="6">
+        <v>42073</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="55" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 051, 052, 053.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="327">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -998,6 +998,12 @@
   </si>
   <si>
     <t>Create form_tags to post multiple checkbox IDs to controllers where update actions are exectued.</t>
+  </si>
+  <si>
+    <t>Handling Exceptions</t>
+  </si>
+  <si>
+    <t>Use public pages, rescue_from, or Rack Middleware via routes to customize exception handling.</t>
   </si>
 </sst>
 </file>
@@ -1061,8 +1067,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1150,7 +1158,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1178,6 +1186,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1205,6 +1214,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1540,7 +1550,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2276,7 +2286,7 @@
         <v>321</v>
       </c>
       <c r="D53" s="6">
-        <v>42073</v>
+        <v>42088</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>322</v>
@@ -2290,15 +2300,24 @@
         <v>323</v>
       </c>
       <c r="D54" s="6">
-        <v>42073</v>
+        <v>42088</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="4">
+      <c r="B55" s="5">
         <v>53</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D55" s="6">
+        <v>42088</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 054.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-2000" yWindow="-21440" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="329">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -1004,6 +1004,12 @@
   </si>
   <si>
     <t>Use public pages, rescue_from, or Rack Middleware via routes to customize exception handling.</t>
+  </si>
+  <si>
+    <t>Debugging Ruby</t>
+  </si>
+  <si>
+    <t>Use Ruby debugger, now byebug in Ruby 2.X, for debugging in Ruby / RoR applications.</t>
   </si>
 </sst>
 </file>
@@ -1550,7 +1556,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2321,8 +2327,17 @@
       </c>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="4">
+      <c r="B56" s="5">
         <v>54</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D56" s="6">
+        <v>42089</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 055.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="331">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -1010,6 +1010,12 @@
   </si>
   <si>
     <t>Use Ruby debugger, now byebug in Ruby 2.X, for debugging in Ruby / RoR applications.</t>
+  </si>
+  <si>
+    <t>Cleaning up views - view logic to helpers, business logic to models, lists to partials with collections.</t>
+  </si>
+  <si>
+    <t>Cleaning Up the View</t>
   </si>
 </sst>
 </file>
@@ -1556,7 +1562,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2341,8 +2347,17 @@
       </c>
     </row>
     <row r="57" spans="2:5">
-      <c r="B57" s="4">
+      <c r="B57" s="5">
         <v>55</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D57" s="6">
+        <v>42097</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="58" spans="2:5">

</xml_diff>

<commit_message>
Watches RailsCasts Episode(s) 056.
</commit_message>
<xml_diff>
--- a/Rails_Casts_Tracking.xlsx
+++ b/Rails_Casts_Tracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="333">
   <si>
     <t>Note some of the syntax is Rails 2</t>
   </si>
@@ -1016,6 +1016,12 @@
   </si>
   <si>
     <t>Cleaning Up the View</t>
+  </si>
+  <si>
+    <t>The Logger</t>
+  </si>
+  <si>
+    <t>Use logger (5 levels) to output messages to log, define your own, rake log:clear to empty out logs.</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1568,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2361,8 +2367,17 @@
       </c>
     </row>
     <row r="58" spans="2:5">
-      <c r="B58" s="4">
+      <c r="B58" s="5">
         <v>56</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D58" s="6">
+        <v>42098</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="2:5">

</xml_diff>